<commit_message>
Updating shapefile to include mobility data per region. However, for some reason this data is not showing up on the map.
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E323B46E-E80D-43A9-B0C2-3A9CC3065438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9F4BE3-6021-4EF1-92F9-E24204DC9B48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="102">
   <si>
     <t>Header or Field Name</t>
   </si>
@@ -295,6 +295,42 @@
   </si>
   <si>
     <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t>Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t>Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t>Parks Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t>Transit Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t>Workplace Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t>Residential Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in residences</t>
   </si>
 </sst>
 </file>
@@ -658,15 +694,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
@@ -1746,9 +1782,111 @@
         <v>15</v>
       </c>
     </row>
+    <row r="59" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added temporal data on oil and gas imports and spatial data on change in household expenditures from Q1 to Q2 for the Indonesia case.
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E692EA-BE4E-4A53-86FF-F189323A27A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,48 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="163">
-  <si>
-    <t xml:space="preserve">Header or Field Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related SD Objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Susceptible Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commonly Used SEIR Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
+  <si>
+    <t>Header or Field Name</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Related SD Objects</t>
+  </si>
+  <si>
+    <t>Context Area</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Required Processing</t>
+  </si>
+  <si>
+    <t>Susceptible Population</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>Commonly Used SEIR Data</t>
+  </si>
+  <si>
+    <t>Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
+  </si>
+  <si>
+    <t>SPop</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
   </si>
   <si>
     <r>
@@ -93,74 +98,74 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
+      <t>https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Basic arithmetic from raw data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santiago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people in hospitals due to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
+    <t>Basic arithmetic from raw data</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Hospitalized Population</t>
+  </si>
+  <si>
+    <t>The number of people in hospitals due to coronavirus.</t>
+  </si>
+  <si>
+    <t>Hpop</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t xml:space="preserve">The number of people in hospital Intensive Care Units (ICU) due to coronavirus. </t>
   </si>
   <si>
-    <t xml:space="preserve">Recovered Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mTotIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
+    <t>Recovered Population</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
+  </si>
+  <si>
+    <t>Rpop</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
+  </si>
+  <si>
+    <t>Measured Current Infected</t>
+  </si>
+  <si>
+    <t>The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
+  </si>
+  <si>
+    <t>mTotIPop</t>
+  </si>
+  <si>
+    <t>mIPop</t>
+  </si>
+  <si>
+    <t>Measured Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
+  </si>
+  <si>
+    <t>True Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>IPop</t>
+  </si>
+  <si>
+    <t>An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
   </si>
   <si>
     <r>
@@ -179,68 +184,68 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
+      <t>NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accumulative Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accumulative deaths attributed to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mInfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalization Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of hospitalization, based on Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HosR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closure Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy and Equipment Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClosureP</t>
+    <t>True Current Infected</t>
+  </si>
+  <si>
+    <t>Accumulative Deaths</t>
+  </si>
+  <si>
+    <t>Accumulative deaths attributed to coronavirus.</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>Measured Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on Measured Current Infected</t>
+  </si>
+  <si>
+    <t>mInfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
+  </si>
+  <si>
+    <t>True Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on True Current Infected</t>
+  </si>
+  <si>
+    <t>InfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of True Current Infected</t>
+  </si>
+  <si>
+    <t>Hospitalization Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of hospitalization, based on Hospitalized Population</t>
+  </si>
+  <si>
+    <t>HosR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
+  </si>
+  <si>
+    <t>Closure Policy</t>
+  </si>
+  <si>
+    <t>Policy and Equipment Data</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
+  </si>
+  <si>
+    <t>ClosureP</t>
   </si>
   <si>
     <r>
@@ -261,137 +266,137 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
+      <t>https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Taking dates of policy changes and converting that to daily policy status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile’s closure policy status, as defined by the Paso a Paso program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currently a placeholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of available ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily number of PCR tests for coronavirus conducted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average temperature in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of SO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCNM in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCT in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CH4 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NOx in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of O3 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM10 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM2.5 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socioeconomic Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro unemployment rate, updated quarterly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RioEmployment</t>
+    <t>Taking dates of policy changes and converting that to daily policy status</t>
+  </si>
+  <si>
+    <t>Chile’s closure policy status, as defined by the Paso a Paso program</t>
+  </si>
+  <si>
+    <t>Currently a placeholder</t>
+  </si>
+  <si>
+    <t>Ventilators</t>
+  </si>
+  <si>
+    <t>Number of available ventilators</t>
+  </si>
+  <si>
+    <t>Vents</t>
+  </si>
+  <si>
+    <t>Placeholder value</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PCR Tests</t>
+  </si>
+  <si>
+    <t>Daily number of PCR tests for coronavirus conducted</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Environmental Data</t>
+  </si>
+  <si>
+    <t>Daily average temperature in the city</t>
+  </si>
+  <si>
+    <t>https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of SO2 in the city</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO2 in the city</t>
+  </si>
+  <si>
+    <t>HCNM</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCNM in the city</t>
+  </si>
+  <si>
+    <t>HCT</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCT in the city</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CH4 in the city</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CO in the city</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO in the city</t>
+  </si>
+  <si>
+    <t>NOx</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NOx in the city</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>Daily average concentration of O3 in the city</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM10 in the city</t>
+  </si>
+  <si>
+    <t>PM2.5</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM2.5 in the city</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Socioeconomic Data</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro unemployment rate, updated quarterly</t>
+  </si>
+  <si>
+    <t>RioEmployment</t>
   </si>
   <si>
     <r>
@@ -411,149 +416,149 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
+      <t>https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil unemployment rate, updated monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BraEmployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gross Domestic Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air Passengers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AirPass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail and Recreation Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in retail and recreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery and Pharmacy Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in Grocery and Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in parks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility for transit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in workplaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in residences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shapefile</t>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Brazil Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Brazil unemployment rate, updated monthly</t>
+  </si>
+  <si>
+    <t>BraEmployment</t>
+  </si>
+  <si>
+    <t>Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
+  </si>
+  <si>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>GDP_Ind</t>
+  </si>
+  <si>
+    <t>Air Passengers</t>
+  </si>
+  <si>
+    <t>Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
+  </si>
+  <si>
+    <t>AirPass</t>
+  </si>
+  <si>
+    <t>Arrivals</t>
+  </si>
+  <si>
+    <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t>Arrivals_Ind</t>
+  </si>
+  <si>
+    <t>Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t>Retail_Mob</t>
+  </si>
+  <si>
+    <t>Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t>Grocery_Mob</t>
+  </si>
+  <si>
+    <t>Parks Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t>Parks_Mob</t>
+  </si>
+  <si>
+    <t>Transit Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t>Transit_Mob</t>
+  </si>
+  <si>
+    <t>Workplace Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t>Workplace_Mob</t>
+  </si>
+  <si>
+    <t>Residential Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in residences</t>
+  </si>
+  <si>
+    <t>Residential_Mob</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>shapefile</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of rain in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pres</t>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
+  </si>
+  <si>
+    <t>Pres</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of barometric pressure in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">SolRad</t>
+    <t>SolRad</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of solar radiance in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Temp</t>
+    <t>Temp</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of temperature in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Humid</t>
+    <t>Humid</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of relative humidity in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindDir</t>
+    <t>WindDir</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind direction (degrees) in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindSpd</t>
+    <t>WindSpd</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind speed in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
@@ -589,20 +594,41 @@
     <t xml:space="preserve">Mean anomaly of PM10 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">PM2_5</t>
+    <t>PM2_5</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of PM2.5 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
+  </si>
+  <si>
+    <t>oil_imports</t>
+  </si>
+  <si>
+    <t>oil and gas imports for each month in Indonesia (Millions USD)</t>
+  </si>
+  <si>
+    <t>https://www.bps.go.id/indicator/8/1754/1/nilai-impor-migas-nonmigas.html</t>
+  </si>
+  <si>
+    <t>houseex</t>
+  </si>
+  <si>
+    <t>% change in household expenditures from Q1 to Q2 in Indonesia</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qkYUf1e_GsEHAW2DR2JUjsuSwkw987v4/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>open in excel, remove spaces and commas from numbers, then use Q1 and Q2 numbers to calculate percent change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -610,22 +636,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -653,7 +664,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -661,95 +672,358 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.98"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,23 +1049,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -801,7 +1075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -825,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -849,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -873,11 +1147,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -886,10 +1160,10 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -899,7 +1173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -921,7 +1195,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -943,11 +1217,11 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -956,17 +1230,17 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -988,11 +1262,11 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1001,10 +1275,10 @@
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1014,7 +1288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1308,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -1054,7 +1328,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1074,20 +1348,20 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -1100,7 +1374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -1120,7 +1394,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1140,11 +1414,11 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1153,10 +1427,10 @@
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1166,7 +1440,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -1186,7 +1460,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1206,7 +1480,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" s="5" customFormat="true" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -1254,7 +1528,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -1276,7 +1550,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -1298,11 +1572,11 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1314,7 +1588,7 @@
       <c r="E25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1324,7 +1598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1346,7 +1620,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1368,7 +1642,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1390,23 +1664,23 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="0" t="s">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1416,7 +1690,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
@@ -1438,7 +1712,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -1460,7 +1734,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1482,11 +1756,11 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -1495,10 +1769,10 @@
       <c r="D33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1508,7 +1782,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
@@ -1530,7 +1804,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
@@ -1543,7 +1817,7 @@
       <c r="D35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" t="s">
         <v>57</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1556,7 +1830,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>54</v>
       </c>
@@ -1569,7 +1843,7 @@
       <c r="D36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" t="s">
         <v>57</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -1578,7 +1852,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
@@ -1591,7 +1865,7 @@
       <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" t="s">
         <v>57</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1600,11 +1874,11 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1613,18 +1887,18 @@
       <c r="D38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1633,10 +1907,10 @@
       <c r="D39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1646,7 +1920,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>62</v>
       </c>
@@ -1659,7 +1933,7 @@
       <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" t="s">
         <v>64</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -1668,11 +1942,11 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1681,18 +1955,18 @@
       <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" t="s">
         <v>69</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1701,10 +1975,10 @@
       <c r="D42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -1714,11 +1988,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1727,10 +2001,10 @@
       <c r="D43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" t="s">
         <v>75</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -1740,11 +2014,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -1753,10 +2027,10 @@
       <c r="D44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -1766,11 +2040,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1779,10 +2053,10 @@
       <c r="D45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -1792,11 +2066,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -1805,10 +2079,10 @@
       <c r="D46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>82</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -1818,11 +2092,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -1831,10 +2105,10 @@
       <c r="D47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -1844,11 +2118,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -1857,10 +2131,10 @@
       <c r="D48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -1870,11 +2144,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1883,10 +2157,10 @@
       <c r="D49" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" t="s">
         <v>88</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -1896,11 +2170,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -1909,10 +2183,10 @@
       <c r="D50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" t="s">
         <v>90</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -1922,11 +2196,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -1935,10 +2209,10 @@
       <c r="D51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" t="s">
         <v>92</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -1948,11 +2222,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -1961,10 +2235,10 @@
       <c r="D52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -1974,11 +2248,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -1987,10 +2261,10 @@
       <c r="D53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -2000,11 +2274,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -2013,10 +2287,10 @@
       <c r="D54" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" t="s">
         <v>101</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -2026,11 +2300,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -2039,10 +2313,10 @@
       <c r="D55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" t="s">
         <v>106</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -2052,28 +2326,28 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" t="s">
         <v>110</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2082,18 +2356,18 @@
       <c r="D57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" t="s">
         <v>113</v>
       </c>
-      <c r="F57" s="0" t="s">
+      <c r="F57" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2102,18 +2376,18 @@
       <c r="D58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" t="s">
         <v>116</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="5" t="s">
@@ -2122,18 +2396,18 @@
       <c r="D59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" t="s">
         <v>119</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>120</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2142,18 +2416,18 @@
       <c r="D60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" t="s">
         <v>122</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -2162,18 +2436,18 @@
       <c r="D61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" t="s">
         <v>125</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -2182,18 +2456,18 @@
       <c r="D62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" t="s">
         <v>128</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -2202,18 +2476,18 @@
       <c r="D63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" t="s">
         <v>131</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>132</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -2222,18 +2496,18 @@
       <c r="D64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" t="s">
         <v>134</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>136</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2242,10 +2516,10 @@
       <c r="D65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" t="s">
         <v>66</v>
       </c>
-      <c r="F65" s="0" t="s">
+      <c r="F65" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -2255,11 +2529,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>136</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2268,10 +2542,10 @@
       <c r="D66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" t="s">
         <v>66</v>
       </c>
-      <c r="F66" s="0" t="s">
+      <c r="F66" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="4" t="s">
@@ -2281,11 +2555,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>136</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2294,10 +2568,10 @@
       <c r="D67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" t="s">
         <v>66</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F67" t="s">
         <v>13</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -2307,11 +2581,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -2320,10 +2594,10 @@
       <c r="D68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" t="s">
         <v>66</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="F68" t="s">
         <v>13</v>
       </c>
       <c r="G68" s="4" t="s">
@@ -2333,11 +2607,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>136</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2346,10 +2620,10 @@
       <c r="D69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" t="s">
         <v>66</v>
       </c>
-      <c r="F69" s="0" t="s">
+      <c r="F69" t="s">
         <v>13</v>
       </c>
       <c r="G69" s="4" t="s">
@@ -2359,11 +2633,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>136</v>
       </c>
       <c r="C70" s="5" t="s">
@@ -2372,10 +2646,10 @@
       <c r="D70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" t="s">
         <v>66</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" t="s">
         <v>13</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -2385,11 +2659,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>149</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>136</v>
       </c>
       <c r="C71" s="5" t="s">
@@ -2398,10 +2672,10 @@
       <c r="D71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" t="s">
         <v>66</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="F71" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="4" t="s">
@@ -2411,11 +2685,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>136</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -2424,10 +2698,10 @@
       <c r="D72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" t="s">
         <v>66</v>
       </c>
-      <c r="F72" s="0" t="s">
+      <c r="F72" t="s">
         <v>13</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -2437,11 +2711,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>136</v>
       </c>
       <c r="C73" s="5" t="s">
@@ -2450,10 +2724,10 @@
       <c r="D73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -2463,11 +2737,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>136</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -2476,10 +2750,10 @@
       <c r="D74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="0" t="s">
+      <c r="F74" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -2489,11 +2763,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>136</v>
       </c>
       <c r="C75" s="5" t="s">
@@ -2502,10 +2776,10 @@
       <c r="D75" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="0" t="s">
+      <c r="F75" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="4" t="s">
@@ -2515,11 +2789,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>136</v>
       </c>
       <c r="C76" s="5" t="s">
@@ -2528,10 +2802,10 @@
       <c r="D76" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" t="s">
         <v>66</v>
       </c>
-      <c r="F76" s="0" t="s">
+      <c r="F76" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="4" t="s">
@@ -2541,11 +2815,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>136</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -2554,10 +2828,10 @@
       <c r="D77" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="0" t="s">
+      <c r="F77" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="4" t="s">
@@ -2567,11 +2841,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>136</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -2580,10 +2854,10 @@
       <c r="D78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="0" t="s">
+      <c r="F78" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="4" t="s">
@@ -2593,11 +2867,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>90</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>136</v>
       </c>
       <c r="C79" s="5" t="s">
@@ -2606,10 +2880,10 @@
       <c r="D79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" t="s">
         <v>66</v>
       </c>
-      <c r="F79" s="0" t="s">
+      <c r="F79" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="4" t="s">
@@ -2619,11 +2893,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>136</v>
       </c>
       <c r="C80" s="5" t="s">
@@ -2632,10 +2906,10 @@
       <c r="D80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E80" s="0" t="s">
+      <c r="E80" t="s">
         <v>66</v>
       </c>
-      <c r="F80" s="0" t="s">
+      <c r="F80" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="4" t="s">
@@ -2645,11 +2919,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>94</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>136</v>
       </c>
       <c r="C81" s="5" t="s">
@@ -2658,10 +2932,10 @@
       <c r="D81" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" t="s">
         <v>66</v>
       </c>
-      <c r="F81" s="0" t="s">
+      <c r="F81" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="4" t="s">
@@ -2671,11 +2945,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" t="s">
         <v>136</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -2684,10 +2958,10 @@
       <c r="D82" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E82" s="0" t="s">
+      <c r="E82" t="s">
         <v>66</v>
       </c>
-      <c r="F82" s="0" t="s">
+      <c r="F82" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="4" t="s">
@@ -2697,45 +2971,93 @@
         <v>138</v>
       </c>
     </row>
+    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing"/>
-    <hyperlink ref="G42" r:id="rId2" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G43" r:id="rId3" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G44" r:id="rId4" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G45" r:id="rId5" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G46" r:id="rId6" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G47" r:id="rId7" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G48" r:id="rId8" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G49" r:id="rId9" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G50" r:id="rId10" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G51" r:id="rId11" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G52" r:id="rId12" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G53" r:id="rId13" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados"/>
-    <hyperlink ref="G65" r:id="rId15" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G66" r:id="rId16" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G67" r:id="rId17" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G68" r:id="rId18" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G69" r:id="rId19" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G70" r:id="rId20" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G71" r:id="rId21" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G72" r:id="rId22" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G73" r:id="rId23" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G74" r:id="rId24" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G75" r:id="rId25" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G76" r:id="rId26" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G77" r:id="rId27" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G78" r:id="rId28" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G79" r:id="rId29" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G80" r:id="rId30" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G81" r:id="rId31" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G82" r:id="rId32" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G42" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G43" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G47" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G48" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G49" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G50" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G51" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G53" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G65" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G66" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G67" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G68" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G69" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G70" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G71" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G72" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G73" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G74" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G75" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G76" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G77" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G78" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G79" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G80" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G81" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G82" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Revert "Merge branch 'SheaLombardo'"
This reverts commit 37cfcd993ddf157f95f6c5341ca7d6f6504a4f75, reversing
changes made to 78fa248432af0837015baec43dd48dc00666eb54.
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E692EA-BE4E-4A53-86FF-F189323A27A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,48 +20,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
-  <si>
-    <t>Header or Field Name</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Related SD Objects</t>
-  </si>
-  <si>
-    <t>Context Area</t>
-  </si>
-  <si>
-    <t>Data Source</t>
-  </si>
-  <si>
-    <t>Required Processing</t>
-  </si>
-  <si>
-    <t>Susceptible Population</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>Commonly Used SEIR Data</t>
-  </si>
-  <si>
-    <t>Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
-  </si>
-  <si>
-    <t>SPop</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="163">
+  <si>
+    <t xml:space="preserve">Header or Field Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related SD Objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susceptible Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commonly Used SEIR Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro</t>
   </si>
   <si>
     <r>
@@ -98,74 +93,74 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
+      <t xml:space="preserve">https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
     </r>
   </si>
   <si>
-    <t>Basic arithmetic from raw data</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Hospitalized Population</t>
-  </si>
-  <si>
-    <t>The number of people in hospitals due to coronavirus.</t>
-  </si>
-  <si>
-    <t>Hpop</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t xml:space="preserve">Basic arithmetic from raw data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitalized Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people in hospitals due to coronavirus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hpop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">The number of people in hospital Intensive Care Units (ICU) due to coronavirus. </t>
   </si>
   <si>
-    <t>Recovered Population</t>
-  </si>
-  <si>
-    <t>The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
-  </si>
-  <si>
-    <t>Rpop</t>
-  </si>
-  <si>
-    <t>The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
-  </si>
-  <si>
-    <t>Measured Current Infected</t>
-  </si>
-  <si>
-    <t>The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
-  </si>
-  <si>
-    <t>mTotIPop</t>
-  </si>
-  <si>
-    <t>mIPop</t>
-  </si>
-  <si>
-    <t>Measured Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t>The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
-  </si>
-  <si>
-    <t>True Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t>IPop</t>
-  </si>
-  <si>
-    <t>An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
+    <t xml:space="preserve">Recovered Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rpop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mTotIPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mIPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
   </si>
   <si>
     <r>
@@ -184,68 +179,68 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
+      <t xml:space="preserve">NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
     </r>
   </si>
   <si>
-    <t>True Current Infected</t>
-  </si>
-  <si>
-    <t>Accumulative Deaths</t>
-  </si>
-  <si>
-    <t>Accumulative deaths attributed to coronavirus.</t>
-  </si>
-  <si>
-    <t>Deaths</t>
-  </si>
-  <si>
-    <t>Measured Infection Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of infection, based on Measured Current Infected</t>
-  </si>
-  <si>
-    <t>mInfectR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
-  </si>
-  <si>
-    <t>True Infection Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of infection, based on True Current Infected</t>
-  </si>
-  <si>
-    <t>InfectR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of True Current Infected</t>
-  </si>
-  <si>
-    <t>Hospitalization Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of hospitalization, based on Hospitalized Population</t>
-  </si>
-  <si>
-    <t>HosR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
-  </si>
-  <si>
-    <t>Closure Policy</t>
-  </si>
-  <si>
-    <t>Policy and Equipment Data</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
-  </si>
-  <si>
-    <t>ClosureP</t>
+    <t xml:space="preserve">True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accumulative Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accumulative deaths attributed to coronavirus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Infection Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of infection, based on Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mInfectR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Infection Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of infection, based on True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InfectR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitalization Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of hospitalization, based on Hospitalized Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HosR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closure Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy and Equipment Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClosureP</t>
   </si>
   <si>
     <r>
@@ -266,137 +261,137 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
+      <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
     </r>
   </si>
   <si>
-    <t>Taking dates of policy changes and converting that to daily policy status</t>
-  </si>
-  <si>
-    <t>Chile’s closure policy status, as defined by the Paso a Paso program</t>
-  </si>
-  <si>
-    <t>Currently a placeholder</t>
-  </si>
-  <si>
-    <t>Ventilators</t>
-  </si>
-  <si>
-    <t>Number of available ventilators</t>
-  </si>
-  <si>
-    <t>Vents</t>
-  </si>
-  <si>
-    <t>Placeholder value</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>PCR Tests</t>
-  </si>
-  <si>
-    <t>Daily number of PCR tests for coronavirus conducted</t>
-  </si>
-  <si>
-    <t>PCR</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Environmental Data</t>
-  </si>
-  <si>
-    <t>Daily average temperature in the city</t>
-  </si>
-  <si>
-    <t>https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
-  </si>
-  <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
-  </si>
-  <si>
-    <t>SO2</t>
-  </si>
-  <si>
-    <t>Daily average concentration of SO2 in the city</t>
-  </si>
-  <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
-  </si>
-  <si>
-    <t>NO2</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NO2 in the city</t>
-  </si>
-  <si>
-    <t>HCNM</t>
-  </si>
-  <si>
-    <t>Daily average concentration of HCNM in the city</t>
-  </si>
-  <si>
-    <t>HCT</t>
-  </si>
-  <si>
-    <t>Daily average concentration of HCT in the city</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>Daily average concentration of CH4 in the city</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>Daily average concentration of CO in the city</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NO in the city</t>
-  </si>
-  <si>
-    <t>NOx</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NOx in the city</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>Daily average concentration of O3 in the city</t>
-  </si>
-  <si>
-    <t>PM10</t>
-  </si>
-  <si>
-    <t>Daily average concentration of PM10 in the city</t>
-  </si>
-  <si>
-    <t>PM2.5</t>
-  </si>
-  <si>
-    <t>Daily average concentration of PM2.5 in the city</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro Unemployment Rate</t>
-  </si>
-  <si>
-    <t>Socioeconomic Data</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro unemployment rate, updated quarterly</t>
-  </si>
-  <si>
-    <t>RioEmployment</t>
+    <t xml:space="preserve">Taking dates of policy changes and converting that to daily policy status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile’s closure policy status, as defined by the Paso a Paso program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently a placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of available ventilators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCR Tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily number of PCR tests for coronavirus conducted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average temperature in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of SO2 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NO2 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCNM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of HCNM in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of HCT in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of CH4 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of CO in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NO in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NOx in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of O3 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of PM10 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of PM2.5 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socioeconomic Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro unemployment rate, updated quarterly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RioEmployment</t>
   </si>
   <si>
     <r>
@@ -416,149 +411,149 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
+      <t xml:space="preserve">https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
     </r>
   </si>
   <si>
-    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t>Brazil Unemployment Rate</t>
-  </si>
-  <si>
-    <t>Brazil unemployment rate, updated monthly</t>
-  </si>
-  <si>
-    <t>BraEmployment</t>
-  </si>
-  <si>
-    <t>Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
-  </si>
-  <si>
-    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t>Gross Domestic Product</t>
-  </si>
-  <si>
-    <t>GDP_Ind</t>
-  </si>
-  <si>
-    <t>Air Passengers</t>
-  </si>
-  <si>
-    <t>Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
-  </si>
-  <si>
-    <t>AirPass</t>
-  </si>
-  <si>
-    <t>Arrivals</t>
-  </si>
-  <si>
-    <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
-  </si>
-  <si>
-    <t>Arrivals_Ind</t>
-  </si>
-  <si>
-    <t>Retail and Recreation Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in retail and recreation</t>
-  </si>
-  <si>
-    <t>Retail_Mob</t>
-  </si>
-  <si>
-    <t>Grocery and Pharmacy Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
-  </si>
-  <si>
-    <t>Grocery_Mob</t>
-  </si>
-  <si>
-    <t>Parks Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in parks</t>
-  </si>
-  <si>
-    <t>Parks_Mob</t>
-  </si>
-  <si>
-    <t>Transit Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility for transit</t>
-  </si>
-  <si>
-    <t>Transit_Mob</t>
-  </si>
-  <si>
-    <t>Workplace Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in workplaces</t>
-  </si>
-  <si>
-    <t>Workplace_Mob</t>
-  </si>
-  <si>
-    <t>Residential Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in residences</t>
-  </si>
-  <si>
-    <t>Residential_Mob</t>
-  </si>
-  <si>
-    <t>Rain</t>
-  </si>
-  <si>
-    <t>shapefile</t>
+    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil unemployment rate, updated monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BraEmployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_Ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Passengers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AirPass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrivals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrivals_Ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parks Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parks_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workplace Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workplace_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in residences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shapefile</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of rain in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
-  </si>
-  <si>
-    <t>Pres</t>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pres</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of barometric pressure in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>SolRad</t>
+    <t xml:space="preserve">SolRad</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of solar radiance in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Temp</t>
+    <t xml:space="preserve">Temp</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of temperature in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Humid</t>
+    <t xml:space="preserve">Humid</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of relative humidity in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>WindDir</t>
+    <t xml:space="preserve">WindDir</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind direction (degrees) in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>WindSpd</t>
+    <t xml:space="preserve">WindSpd</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind speed in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
@@ -594,41 +589,20 @@
     <t xml:space="preserve">Mean anomaly of PM10 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>PM2_5</t>
+    <t xml:space="preserve">PM2_5</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of PM2.5 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
-  </si>
-  <si>
-    <t>oil_imports</t>
-  </si>
-  <si>
-    <t>oil and gas imports for each month in Indonesia (Millions USD)</t>
-  </si>
-  <si>
-    <t>https://www.bps.go.id/indicator/8/1754/1/nilai-impor-migas-nonmigas.html</t>
-  </si>
-  <si>
-    <t>houseex</t>
-  </si>
-  <si>
-    <t>% change in household expenditures from Q1 to Q2 in Indonesia</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1qkYUf1e_GsEHAW2DR2JUjsuSwkw987v4/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>open in excel, remove spaces and commas from numbers, then use Q1 and Q2 numbers to calculate percent change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -636,7 +610,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -664,7 +653,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -672,358 +661,95 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="48" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1049,23 +775,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1075,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1147,11 +873,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1160,10 +886,10 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1173,7 +899,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +921,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1217,11 +943,11 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1230,17 +956,17 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1262,11 +988,11 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1275,10 +1001,10 @@
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1288,7 +1014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1308,7 +1034,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -1328,7 +1054,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1348,20 +1074,20 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -1374,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -1394,7 +1120,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1414,11 +1140,11 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1427,10 +1153,10 @@
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1440,7 +1166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1186,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1480,7 +1206,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="21" s="5" customFormat="true" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -1506,7 +1232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -1528,7 +1254,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -1550,7 +1276,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -1572,11 +1298,11 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1588,7 +1314,7 @@
       <c r="E25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1598,7 +1324,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1620,7 +1346,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1642,7 +1368,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1664,23 +1390,23 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1690,7 +1416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
@@ -1712,7 +1438,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -1734,7 +1460,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1756,11 +1482,11 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -1769,10 +1495,10 @@
       <c r="D33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1782,7 +1508,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
@@ -1804,7 +1530,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="35" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
@@ -1817,7 +1543,7 @@
       <c r="D35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1830,7 +1556,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>54</v>
       </c>
@@ -1843,7 +1569,7 @@
       <c r="D36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -1852,7 +1578,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
@@ -1865,7 +1591,7 @@
       <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1874,11 +1600,11 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1887,18 +1613,18 @@
       <c r="D38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1907,10 +1633,10 @@
       <c r="D39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1920,7 +1646,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>62</v>
       </c>
@@ -1933,7 +1659,7 @@
       <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="0" t="s">
         <v>64</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -1942,11 +1668,11 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1955,18 +1681,18 @@
       <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1975,10 +1701,10 @@
       <c r="D42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -1988,11 +1714,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -2001,10 +1727,10 @@
       <c r="D43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -2014,11 +1740,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2027,10 +1753,10 @@
       <c r="D44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -2040,11 +1766,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2053,10 +1779,10 @@
       <c r="D45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -2066,11 +1792,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2079,10 +1805,10 @@
       <c r="D46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -2092,11 +1818,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2105,10 +1831,10 @@
       <c r="D47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -2118,11 +1844,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -2131,10 +1857,10 @@
       <c r="D48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -2144,11 +1870,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -2157,10 +1883,10 @@
       <c r="D49" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -2170,11 +1896,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2183,10 +1909,10 @@
       <c r="D50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -2196,11 +1922,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -2209,10 +1935,10 @@
       <c r="D51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -2222,11 +1948,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -2235,10 +1961,10 @@
       <c r="D52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -2248,11 +1974,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -2261,10 +1987,10 @@
       <c r="D53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -2274,11 +2000,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -2287,10 +2013,10 @@
       <c r="D54" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -2300,11 +2026,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -2313,10 +2039,10 @@
       <c r="D55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -2326,28 +2052,28 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2356,18 +2082,18 @@
       <c r="D57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2376,18 +2102,18 @@
       <c r="D58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="0" t="s">
         <v>116</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="5" t="s">
@@ -2396,18 +2122,18 @@
       <c r="D59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="0" t="s">
         <v>119</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2416,18 +2142,18 @@
       <c r="D60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="0" t="s">
         <v>122</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -2436,18 +2162,18 @@
       <c r="D61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="0" t="s">
         <v>125</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="62" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -2456,18 +2182,18 @@
       <c r="D62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="0" t="s">
         <v>128</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -2476,18 +2202,18 @@
       <c r="D63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="0" t="s">
         <v>131</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -2496,18 +2222,18 @@
       <c r="D64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="0" t="s">
         <v>134</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2516,10 +2242,10 @@
       <c r="D65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -2529,11 +2255,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="66" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2542,10 +2268,10 @@
       <c r="D66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="4" t="s">
@@ -2555,11 +2281,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="67" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2568,10 +2294,10 @@
       <c r="D67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -2581,11 +2307,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="68" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -2594,10 +2320,10 @@
       <c r="D68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G68" s="4" t="s">
@@ -2607,11 +2333,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="69" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2620,10 +2346,10 @@
       <c r="D69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G69" s="4" t="s">
@@ -2633,11 +2359,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="70" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C70" s="5" t="s">
@@ -2646,10 +2372,10 @@
       <c r="D70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -2659,11 +2385,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="71" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C71" s="5" t="s">
@@ -2672,10 +2398,10 @@
       <c r="D71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="4" t="s">
@@ -2685,11 +2411,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="72" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -2698,10 +2424,10 @@
       <c r="D72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -2711,11 +2437,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C73" s="5" t="s">
@@ -2724,10 +2450,10 @@
       <c r="D73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -2737,11 +2463,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -2750,10 +2476,10 @@
       <c r="D74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -2763,11 +2489,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="75" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C75" s="5" t="s">
@@ -2776,10 +2502,10 @@
       <c r="D75" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="4" t="s">
@@ -2789,11 +2515,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="76" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C76" s="5" t="s">
@@ -2802,10 +2528,10 @@
       <c r="D76" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="4" t="s">
@@ -2815,11 +2541,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="77" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -2828,10 +2554,10 @@
       <c r="D77" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="4" t="s">
@@ -2841,11 +2567,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="78" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -2854,10 +2580,10 @@
       <c r="D78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="4" t="s">
@@ -2867,11 +2593,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="79" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C79" s="5" t="s">
@@ -2880,10 +2606,10 @@
       <c r="D79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="4" t="s">
@@ -2893,11 +2619,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="80" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C80" s="5" t="s">
@@ -2906,10 +2632,10 @@
       <c r="D80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="4" t="s">
@@ -2919,11 +2645,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="81" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C81" s="5" t="s">
@@ -2932,10 +2658,10 @@
       <c r="D81" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="4" t="s">
@@ -2945,11 +2671,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="82" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -2958,10 +2684,10 @@
       <c r="D82" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="4" t="s">
@@ -2971,93 +2697,45 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>163</v>
-      </c>
-      <c r="B83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>166</v>
-      </c>
-      <c r="B84" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G42" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G43" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G47" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G48" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G49" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G50" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G51" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G53" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G65" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G66" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G67" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G68" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G69" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G70" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G71" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G72" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G73" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G74" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G75" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G76" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G77" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G78" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G79" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G80" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G81" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G82" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing"/>
+    <hyperlink ref="G42" r:id="rId2" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G43" r:id="rId3" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G44" r:id="rId4" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G45" r:id="rId5" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G46" r:id="rId6" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G47" r:id="rId7" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G48" r:id="rId8" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G49" r:id="rId9" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G50" r:id="rId10" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G51" r:id="rId11" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G52" r:id="rId12" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G53" r:id="rId13" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados"/>
+    <hyperlink ref="G65" r:id="rId15" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G66" r:id="rId16" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G67" r:id="rId17" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G68" r:id="rId18" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G69" r:id="rId19" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G70" r:id="rId20" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G71" r:id="rId21" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G72" r:id="rId22" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G73" r:id="rId23" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G74" r:id="rId24" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G75" r:id="rId25" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G76" r:id="rId26" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G77" r:id="rId27" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G78" r:id="rId28" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G79" r:id="rId29" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G80" r:id="rId30" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G81" r:id="rId31" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G82" r:id="rId32" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
   </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adding back in previous addition of change in household expenditure
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389CE7A6-1009-4E43-9046-6F75B0F04CD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,48 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="163">
-  <si>
-    <t xml:space="preserve">Header or Field Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related SD Objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Susceptible Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commonly Used SEIR Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="168">
+  <si>
+    <t>Header or Field Name</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Related SD Objects</t>
+  </si>
+  <si>
+    <t>Context Area</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Required Processing</t>
+  </si>
+  <si>
+    <t>Susceptible Population</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>Commonly Used SEIR Data</t>
+  </si>
+  <si>
+    <t>Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
+  </si>
+  <si>
+    <t>SPop</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
   </si>
   <si>
     <r>
@@ -93,74 +98,74 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
+      <t>https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Basic arithmetic from raw data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santiago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people in hospitals due to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
+    <t>Basic arithmetic from raw data</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Hospitalized Population</t>
+  </si>
+  <si>
+    <t>The number of people in hospitals due to coronavirus.</t>
+  </si>
+  <si>
+    <t>Hpop</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t xml:space="preserve">The number of people in hospital Intensive Care Units (ICU) due to coronavirus. </t>
   </si>
   <si>
-    <t xml:space="preserve">Recovered Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mTotIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
+    <t>Recovered Population</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
+  </si>
+  <si>
+    <t>Rpop</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
+  </si>
+  <si>
+    <t>Measured Current Infected</t>
+  </si>
+  <si>
+    <t>The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
+  </si>
+  <si>
+    <t>mTotIPop</t>
+  </si>
+  <si>
+    <t>mIPop</t>
+  </si>
+  <si>
+    <t>Measured Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
+  </si>
+  <si>
+    <t>True Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>IPop</t>
+  </si>
+  <si>
+    <t>An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
   </si>
   <si>
     <r>
@@ -179,68 +184,68 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
+      <t>NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accumulative Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accumulative deaths attributed to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mInfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalization Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of hospitalization, based on Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HosR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closure Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy and Equipment Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClosureP</t>
+    <t>True Current Infected</t>
+  </si>
+  <si>
+    <t>Accumulative Deaths</t>
+  </si>
+  <si>
+    <t>Accumulative deaths attributed to coronavirus.</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>Measured Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on Measured Current Infected</t>
+  </si>
+  <si>
+    <t>mInfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
+  </si>
+  <si>
+    <t>True Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on True Current Infected</t>
+  </si>
+  <si>
+    <t>InfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of True Current Infected</t>
+  </si>
+  <si>
+    <t>Hospitalization Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of hospitalization, based on Hospitalized Population</t>
+  </si>
+  <si>
+    <t>HosR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
+  </si>
+  <si>
+    <t>Closure Policy</t>
+  </si>
+  <si>
+    <t>Policy and Equipment Data</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
+  </si>
+  <si>
+    <t>ClosureP</t>
   </si>
   <si>
     <r>
@@ -261,137 +266,137 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
+      <t>https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Taking dates of policy changes and converting that to daily policy status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile’s closure policy status, as defined by the Paso a Paso program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currently a placeholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of available ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily number of PCR tests for coronavirus conducted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average temperature in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of SO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCNM in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCT in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CH4 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NOx in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of O3 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM10 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM2.5 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socioeconomic Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro unemployment rate, updated quarterly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RioEmployment</t>
+    <t>Taking dates of policy changes and converting that to daily policy status</t>
+  </si>
+  <si>
+    <t>Chile’s closure policy status, as defined by the Paso a Paso program</t>
+  </si>
+  <si>
+    <t>Currently a placeholder</t>
+  </si>
+  <si>
+    <t>Ventilators</t>
+  </si>
+  <si>
+    <t>Number of available ventilators</t>
+  </si>
+  <si>
+    <t>Vents</t>
+  </si>
+  <si>
+    <t>Placeholder value</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PCR Tests</t>
+  </si>
+  <si>
+    <t>Daily number of PCR tests for coronavirus conducted</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Environmental Data</t>
+  </si>
+  <si>
+    <t>Daily average temperature in the city</t>
+  </si>
+  <si>
+    <t>https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of SO2 in the city</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO2 in the city</t>
+  </si>
+  <si>
+    <t>HCNM</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCNM in the city</t>
+  </si>
+  <si>
+    <t>HCT</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCT in the city</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CH4 in the city</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CO in the city</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO in the city</t>
+  </si>
+  <si>
+    <t>NOx</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NOx in the city</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>Daily average concentration of O3 in the city</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM10 in the city</t>
+  </si>
+  <si>
+    <t>PM2.5</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM2.5 in the city</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Socioeconomic Data</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro unemployment rate, updated quarterly</t>
+  </si>
+  <si>
+    <t>RioEmployment</t>
   </si>
   <si>
     <r>
@@ -411,149 +416,149 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
+      <t>https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil unemployment rate, updated monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BraEmployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gross Domestic Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air Passengers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AirPass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail and Recreation Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in retail and recreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery and Pharmacy Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in Grocery and Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in parks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility for transit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in workplaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in residences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shapefile</t>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Brazil Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Brazil unemployment rate, updated monthly</t>
+  </si>
+  <si>
+    <t>BraEmployment</t>
+  </si>
+  <si>
+    <t>Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
+  </si>
+  <si>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>GDP_Ind</t>
+  </si>
+  <si>
+    <t>Air Passengers</t>
+  </si>
+  <si>
+    <t>Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
+  </si>
+  <si>
+    <t>AirPass</t>
+  </si>
+  <si>
+    <t>Arrivals</t>
+  </si>
+  <si>
+    <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t>Arrivals_Ind</t>
+  </si>
+  <si>
+    <t>Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t>Retail_Mob</t>
+  </si>
+  <si>
+    <t>Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t>Grocery_Mob</t>
+  </si>
+  <si>
+    <t>Parks Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t>Parks_Mob</t>
+  </si>
+  <si>
+    <t>Transit Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t>Transit_Mob</t>
+  </si>
+  <si>
+    <t>Workplace Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t>Workplace_Mob</t>
+  </si>
+  <si>
+    <t>Residential Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in residences</t>
+  </si>
+  <si>
+    <t>Residential_Mob</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>shapefile</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of rain in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pres</t>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
+  </si>
+  <si>
+    <t>Pres</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of barometric pressure in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">SolRad</t>
+    <t>SolRad</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of solar radiance in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Temp</t>
+    <t>Temp</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of temperature in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Humid</t>
+    <t>Humid</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of relative humidity in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindDir</t>
+    <t>WindDir</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind direction (degrees) in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindSpd</t>
+    <t>WindSpd</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind speed in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
@@ -589,20 +594,32 @@
     <t xml:space="preserve">Mean anomaly of PM10 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">PM2_5</t>
+    <t>PM2_5</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of PM2.5 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
+  </si>
+  <si>
+    <t>houseex</t>
+  </si>
+  <si>
+    <t>change in house hould expenditures from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>remove commas from data and calculate percent change from raw Q1 and Q2 numbers</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -610,22 +627,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -653,7 +655,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -661,95 +663,358 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.98"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,23 +1040,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -801,7 +1066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -825,7 +1090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -849,7 +1114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" s="5" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -873,11 +1138,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -886,10 +1151,10 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -899,7 +1164,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -921,7 +1186,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -943,11 +1208,11 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -956,17 +1221,17 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -988,11 +1253,11 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1001,10 +1266,10 @@
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1014,7 +1279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1299,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -1054,7 +1319,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1074,20 +1339,20 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -1100,7 +1365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -1120,7 +1385,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1140,11 +1405,11 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1153,10 +1418,10 @@
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1166,7 +1431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -1186,7 +1451,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1206,7 +1471,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" s="5" customFormat="true" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -1254,7 +1519,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -1276,7 +1541,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -1298,11 +1563,11 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1314,7 +1579,7 @@
       <c r="E25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1324,7 +1589,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1346,7 +1611,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1368,7 +1633,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1390,23 +1655,23 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="0" t="s">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1416,7 +1681,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
@@ -1438,7 +1703,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -1460,7 +1725,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1482,11 +1747,11 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -1495,10 +1760,10 @@
       <c r="D33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1508,7 +1773,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
@@ -1530,7 +1795,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" s="5" customFormat="true" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
@@ -1543,7 +1808,7 @@
       <c r="D35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" t="s">
         <v>57</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1556,7 +1821,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>54</v>
       </c>
@@ -1569,7 +1834,7 @@
       <c r="D36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" t="s">
         <v>57</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -1578,7 +1843,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
@@ -1591,7 +1856,7 @@
       <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" t="s">
         <v>57</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1600,11 +1865,11 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1613,18 +1878,18 @@
       <c r="D38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1633,10 +1898,10 @@
       <c r="D39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1646,7 +1911,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>62</v>
       </c>
@@ -1659,7 +1924,7 @@
       <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" t="s">
         <v>64</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -1668,11 +1933,11 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1681,18 +1946,18 @@
       <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" t="s">
         <v>69</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1701,10 +1966,10 @@
       <c r="D42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -1714,11 +1979,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1727,10 +1992,10 @@
       <c r="D43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" t="s">
         <v>75</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -1740,11 +2005,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -1753,10 +2018,10 @@
       <c r="D44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -1766,11 +2031,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1779,10 +2044,10 @@
       <c r="D45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -1792,11 +2057,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -1805,10 +2070,10 @@
       <c r="D46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>82</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -1818,11 +2083,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -1831,10 +2096,10 @@
       <c r="D47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -1844,11 +2109,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -1857,10 +2122,10 @@
       <c r="D48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -1870,11 +2135,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1883,10 +2148,10 @@
       <c r="D49" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" t="s">
         <v>88</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -1896,11 +2161,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -1909,10 +2174,10 @@
       <c r="D50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" t="s">
         <v>90</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -1922,11 +2187,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -1935,10 +2200,10 @@
       <c r="D51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" t="s">
         <v>92</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -1948,11 +2213,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -1961,10 +2226,10 @@
       <c r="D52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -1974,11 +2239,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -1987,10 +2252,10 @@
       <c r="D53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -2000,11 +2265,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -2013,10 +2278,10 @@
       <c r="D54" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" t="s">
         <v>101</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -2026,11 +2291,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -2039,10 +2304,10 @@
       <c r="D55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" t="s">
         <v>106</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -2052,28 +2317,28 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" t="s">
         <v>110</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2082,18 +2347,18 @@
       <c r="D57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" t="s">
         <v>113</v>
       </c>
-      <c r="F57" s="0" t="s">
+      <c r="F57" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2102,18 +2367,18 @@
       <c r="D58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" t="s">
         <v>116</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="5" t="s">
@@ -2122,18 +2387,18 @@
       <c r="D59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" t="s">
         <v>119</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>120</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2142,18 +2407,18 @@
       <c r="D60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" t="s">
         <v>122</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -2162,18 +2427,18 @@
       <c r="D61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" t="s">
         <v>125</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -2182,18 +2447,18 @@
       <c r="D62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" t="s">
         <v>128</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -2202,18 +2467,18 @@
       <c r="D63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" t="s">
         <v>131</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>132</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -2222,18 +2487,18 @@
       <c r="D64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" t="s">
         <v>134</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>136</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2242,10 +2507,10 @@
       <c r="D65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" t="s">
         <v>66</v>
       </c>
-      <c r="F65" s="0" t="s">
+      <c r="F65" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -2255,11 +2520,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>136</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2268,10 +2533,10 @@
       <c r="D66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" t="s">
         <v>66</v>
       </c>
-      <c r="F66" s="0" t="s">
+      <c r="F66" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="4" t="s">
@@ -2281,11 +2546,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>136</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2294,10 +2559,10 @@
       <c r="D67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" t="s">
         <v>66</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F67" t="s">
         <v>13</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -2307,11 +2572,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -2320,10 +2585,10 @@
       <c r="D68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" t="s">
         <v>66</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="F68" t="s">
         <v>13</v>
       </c>
       <c r="G68" s="4" t="s">
@@ -2333,11 +2598,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>136</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2346,10 +2611,10 @@
       <c r="D69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" t="s">
         <v>66</v>
       </c>
-      <c r="F69" s="0" t="s">
+      <c r="F69" t="s">
         <v>13</v>
       </c>
       <c r="G69" s="4" t="s">
@@ -2359,11 +2624,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>136</v>
       </c>
       <c r="C70" s="5" t="s">
@@ -2372,10 +2637,10 @@
       <c r="D70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" t="s">
         <v>66</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" t="s">
         <v>13</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -2385,11 +2650,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>149</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>136</v>
       </c>
       <c r="C71" s="5" t="s">
@@ -2398,10 +2663,10 @@
       <c r="D71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" t="s">
         <v>66</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="F71" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="4" t="s">
@@ -2411,11 +2676,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>136</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -2424,10 +2689,10 @@
       <c r="D72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" t="s">
         <v>66</v>
       </c>
-      <c r="F72" s="0" t="s">
+      <c r="F72" t="s">
         <v>13</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -2437,11 +2702,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>136</v>
       </c>
       <c r="C73" s="5" t="s">
@@ -2450,10 +2715,10 @@
       <c r="D73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -2463,11 +2728,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>136</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -2476,10 +2741,10 @@
       <c r="D74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="0" t="s">
+      <c r="F74" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -2489,11 +2754,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>136</v>
       </c>
       <c r="C75" s="5" t="s">
@@ -2502,10 +2767,10 @@
       <c r="D75" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="0" t="s">
+      <c r="F75" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="4" t="s">
@@ -2515,11 +2780,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>136</v>
       </c>
       <c r="C76" s="5" t="s">
@@ -2528,10 +2793,10 @@
       <c r="D76" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" t="s">
         <v>66</v>
       </c>
-      <c r="F76" s="0" t="s">
+      <c r="F76" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="4" t="s">
@@ -2541,11 +2806,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>136</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -2554,10 +2819,10 @@
       <c r="D77" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="0" t="s">
+      <c r="F77" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="4" t="s">
@@ -2567,11 +2832,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>136</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -2580,10 +2845,10 @@
       <c r="D78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="0" t="s">
+      <c r="F78" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="4" t="s">
@@ -2593,11 +2858,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>90</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>136</v>
       </c>
       <c r="C79" s="5" t="s">
@@ -2606,10 +2871,10 @@
       <c r="D79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" t="s">
         <v>66</v>
       </c>
-      <c r="F79" s="0" t="s">
+      <c r="F79" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="4" t="s">
@@ -2619,11 +2884,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>136</v>
       </c>
       <c r="C80" s="5" t="s">
@@ -2632,10 +2897,10 @@
       <c r="D80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E80" s="0" t="s">
+      <c r="E80" t="s">
         <v>66</v>
       </c>
-      <c r="F80" s="0" t="s">
+      <c r="F80" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="4" t="s">
@@ -2645,11 +2910,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>94</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>136</v>
       </c>
       <c r="C81" s="5" t="s">
@@ -2658,10 +2923,10 @@
       <c r="D81" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" t="s">
         <v>66</v>
       </c>
-      <c r="F81" s="0" t="s">
+      <c r="F81" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="4" t="s">
@@ -2671,11 +2936,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" t="s">
         <v>136</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -2684,10 +2949,10 @@
       <c r="D82" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E82" s="0" t="s">
+      <c r="E82" t="s">
         <v>66</v>
       </c>
-      <c r="F82" s="0" t="s">
+      <c r="F82" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="4" t="s">
@@ -2697,45 +2962,70 @@
         <v>138</v>
       </c>
     </row>
+    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing"/>
-    <hyperlink ref="G42" r:id="rId2" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G43" r:id="rId3" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G44" r:id="rId4" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G45" r:id="rId5" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G46" r:id="rId6" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G47" r:id="rId7" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G48" r:id="rId8" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G49" r:id="rId9" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G50" r:id="rId10" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G51" r:id="rId11" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G52" r:id="rId12" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G53" r:id="rId13" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados"/>
-    <hyperlink ref="G65" r:id="rId15" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G66" r:id="rId16" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G67" r:id="rId17" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G68" r:id="rId18" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G69" r:id="rId19" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G70" r:id="rId20" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G71" r:id="rId21" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G72" r:id="rId22" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G73" r:id="rId23" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G74" r:id="rId24" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G75" r:id="rId25" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G76" r:id="rId26" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G77" r:id="rId27" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G78" r:id="rId28" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G79" r:id="rId29" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G80" r:id="rId30" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G81" r:id="rId31" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G82" r:id="rId32" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G35" r:id="rId1" display="https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G42" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G43" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G47" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G48" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G49" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G50" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G51" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G53" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G54" r:id="rId14" display="https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G65" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G66" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G67" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G68" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G69" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G70" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G71" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G72" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G73" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G74" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G75" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G76" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G77" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G78" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G79" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G80" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G81" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G82" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adding back in previous addition of temporal oil import data
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389CE7A6-1009-4E43-9046-6F75B0F04CD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1425D80C-C0E6-49BB-8DDF-4999164E6750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
   <si>
     <t>Header or Field Name</t>
   </si>
@@ -613,6 +613,15 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
+  </si>
+  <si>
+    <t>oil_imports</t>
+  </si>
+  <si>
+    <t>monthly oil and gas imports</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -996,11 +1005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2986,6 +2995,29 @@
       </c>
       <c r="H83" s="1" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new temporal and spatial economic data to the Indonesia case
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1425D80C-C0E6-49BB-8DDF-4999164E6750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08940D3B-6458-418B-91B6-06BF1B7B841A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="201">
   <si>
     <t>Header or Field Name</t>
   </si>
@@ -622,6 +622,96 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>consumex</t>
+  </si>
+  <si>
+    <t>govex</t>
+  </si>
+  <si>
+    <t>netex</t>
+  </si>
+  <si>
+    <t>GDRP</t>
+  </si>
+  <si>
+    <t>Consumtion Expenditure LNPRT % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>Government Consumption Expenditure % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>Net Export % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gross Domestic Regional Expenditure % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>https://www.bps.go.id/indicator/171/533/1/pdrb-adh-konstan-menurut-pengeluaran-2010-100-.html</t>
+  </si>
+  <si>
+    <t>household_ex</t>
+  </si>
+  <si>
+    <t>Consumtion_ex</t>
+  </si>
+  <si>
+    <t>gov_ex</t>
+  </si>
+  <si>
+    <t>net_ex</t>
+  </si>
+  <si>
+    <t>GDP_manu</t>
+  </si>
+  <si>
+    <t>GDP_cons</t>
+  </si>
+  <si>
+    <t>GDP_retail</t>
+  </si>
+  <si>
+    <t>GDP_IT</t>
+  </si>
+  <si>
+    <t>GDP_social</t>
+  </si>
+  <si>
+    <t>GDP_food</t>
+  </si>
+  <si>
+    <t>Household Expenditures</t>
+  </si>
+  <si>
+    <t>Consumtion Expenditure LNPRT</t>
+  </si>
+  <si>
+    <t>Government Consumption Expenditure</t>
+  </si>
+  <si>
+    <t>Net Exports</t>
+  </si>
+  <si>
+    <t>Manufacturing GDP</t>
+  </si>
+  <si>
+    <t>Construction GDP</t>
+  </si>
+  <si>
+    <t>Retail and Vehicle Repair GDP</t>
+  </si>
+  <si>
+    <t>Information and Communication GDP</t>
+  </si>
+  <si>
+    <t>Health and Social Work GDP</t>
+  </si>
+  <si>
+    <t>Accomodation and Food Service GDP</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -1005,18 +1095,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="58.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="48" style="1" customWidth="1"/>
@@ -2991,13 +3081,13 @@
         <v>18</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -3018,6 +3108,340 @@
       </c>
       <c r="G84" s="1" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" t="s">
+        <v>175</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D86" t="s">
+        <v>176</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>173</v>
+      </c>
+      <c r="B87" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" t="s">
+        <v>178</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>189</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3056,7 +3480,7 @@
     <hyperlink ref="G82" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId33"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added in new Indonesian economic data and fixed bug in Indonesian decision rules
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08940D3B-6458-418B-91B6-06BF1B7B841A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A72DA8-F6AC-4230-BEFD-10E4381F9E71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="212">
   <si>
     <t>Header or Field Name</t>
   </si>
@@ -712,6 +712,39 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>FTT</t>
+  </si>
+  <si>
+    <t>removed commas</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1y9htQ6XCSQ97M_PmUNJv8V2F0fNSPs5F?usp=sharing</t>
+  </si>
+  <si>
+    <t>stock_index</t>
+  </si>
+  <si>
+    <t>closing composite stock index (IDX</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/12brQyMurZj1aQp8jScS5RBKPRe41q-CG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>added in rows for missing dates (weekends and holidays)</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>Farmer Terms of Trade (have values for each of the 5 provinces)</t>
+  </si>
+  <si>
+    <t>poverty rate</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1gL2MblktoxtyZoEX1UjuB_B8hVqO4TFT/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -1095,11 +1128,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
+      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1165,7 +1198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1213,7 +1246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1307,7 +1340,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1688,7 +1721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1710,7 +1743,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1732,7 +1765,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1872,7 +1905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
@@ -2453,7 +2486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -2473,7 +2506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -2493,7 +2526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -3306,7 +3339,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -3398,7 +3431,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -3421,7 +3454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>189</v>
       </c>
@@ -3442,6 +3475,84 @@
       </c>
       <c r="G98" s="1" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new transportation data to Indonesia
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944D8965-BFFD-49DB-8D6F-4257D5D1A174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$H$99</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,454 +28,454 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="225">
-  <si>
-    <t xml:space="preserve">Header or Field Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related SD Objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Susceptible Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commonly Used SEIR Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic from raw data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalized Population</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="260">
+  <si>
+    <t>Header or Field Name</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Related SD Objects</t>
+  </si>
+  <si>
+    <t>Context Area</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Required Processing</t>
+  </si>
+  <si>
+    <t>Susceptible Population</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>Commonly Used SEIR Data</t>
+  </si>
+  <si>
+    <t>Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
+  </si>
+  <si>
+    <t>SPop</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv</t>
+  </si>
+  <si>
+    <t>Basic arithmetic from raw data</t>
+  </si>
+  <si>
+    <t>Hospitalized Population</t>
   </si>
   <si>
     <t xml:space="preserve">The number of people in hospital Intensive Care Units (ICU) due to coronavirus. </t>
   </si>
   <si>
-    <t xml:space="preserve">Hpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovered Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of active cases, as defined by the Ministry of Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mTotIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mIPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder: Samples from a normal distribution that ses the Measured Unhospitalized Infected from one week in the future as the mean and 0.25*that value as the standard deviation
+    <t>Hpop</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Recovered Population</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
+  </si>
+  <si>
+    <t>Rpop</t>
+  </si>
+  <si>
+    <t>Measured Current Infected</t>
+  </si>
+  <si>
+    <t>The number of active cases, as defined by the Ministry of Health</t>
+  </si>
+  <si>
+    <t>mTotIPop</t>
+  </si>
+  <si>
+    <t>Measured Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
+  </si>
+  <si>
+    <t>mIPop</t>
+  </si>
+  <si>
+    <t>True Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t>An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
+  </si>
+  <si>
+    <t>IPop</t>
+  </si>
+  <si>
+    <t>Placeholder: Samples from a normal distribution that ses the Measured Unhospitalized Infected from one week in the future as the mean and 0.25*that value as the standard deviation
 NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
   </si>
   <si>
-    <t xml:space="preserve">Accumulative Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accumulative deaths attributed to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum across regions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mInfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Infection Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of infection, based on True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InfectR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalization Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily rate of hospitalization, based on Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HosR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closure Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy and Equipment Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile’s closure policy status, as defined by the Paso a Paso program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClosureP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder: need to identify actual history, varies from province to province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of available ventilators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily number of PCR tests for coronavirus conducted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air Passengers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socioeconomic Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AirPass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum across destination regions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True Current Infected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currently a placeholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gross Domestic Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrivals_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail and Recreation Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in retail and recreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery and Pharmacy Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in Grocery and Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in parks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parks_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility for transit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in workplaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workplace_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential Mobility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent change from baseline for mobility in residences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential_Mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">houseex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shapefile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">change in house hould expenditures from Q1 to Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.bps.go.id/indicator/171/533/1/pdrb-adh-konstan-menurut-pengeluaran-2010-100-.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remove commas from data and calculate percent change from raw Q1 and Q2 numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oil_imports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthly oil and gas imports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">na</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumtion Expenditure LNPRT % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">govex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government Consumption Expenditure % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">netex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net Export % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDRP</t>
+    <t>Accumulative Deaths</t>
+  </si>
+  <si>
+    <t>Accumulative deaths attributed to coronavirus.</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto14</t>
+  </si>
+  <si>
+    <t>Sum across regions</t>
+  </si>
+  <si>
+    <t>Measured Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on Measured Current Infected</t>
+  </si>
+  <si>
+    <t>mInfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
+  </si>
+  <si>
+    <t>True Infection Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of infection, based on True Current Infected</t>
+  </si>
+  <si>
+    <t>InfectR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of True Current Infected</t>
+  </si>
+  <si>
+    <t>Hospitalization Rate</t>
+  </si>
+  <si>
+    <t>Daily rate of hospitalization, based on Hospitalized Population</t>
+  </si>
+  <si>
+    <t>HosR</t>
+  </si>
+  <si>
+    <t>Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
+  </si>
+  <si>
+    <t>Closure Policy</t>
+  </si>
+  <si>
+    <t>Policy and Equipment Data</t>
+  </si>
+  <si>
+    <t>Chile’s closure policy status, as defined by the Paso a Paso program</t>
+  </si>
+  <si>
+    <t>ClosureP</t>
+  </si>
+  <si>
+    <t>Placeholder: need to identify actual history, varies from province to province</t>
+  </si>
+  <si>
+    <t>Ventilators</t>
+  </si>
+  <si>
+    <t>Number of available ventilators</t>
+  </si>
+  <si>
+    <t>Vents</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20</t>
+  </si>
+  <si>
+    <t>PCR Tests</t>
+  </si>
+  <si>
+    <t>Daily number of PCR tests for coronavirus conducted</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7</t>
+  </si>
+  <si>
+    <t>Air Passengers</t>
+  </si>
+  <si>
+    <t>Socioeconomic Data</t>
+  </si>
+  <si>
+    <t>Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
+  </si>
+  <si>
+    <t>AirPass</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40</t>
+  </si>
+  <si>
+    <t>Sum across destination regions</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>True Current Infected</t>
+  </si>
+  <si>
+    <t>Currently a placeholder</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>GDP_Ind</t>
+  </si>
+  <si>
+    <t>Arrivals</t>
+  </si>
+  <si>
+    <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t>Arrivals_Ind</t>
+  </si>
+  <si>
+    <t>Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t>Environmental Data</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t>Retail_Mob</t>
+  </si>
+  <si>
+    <t>Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t>Grocery_Mob</t>
+  </si>
+  <si>
+    <t>Parks Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t>Parks_Mob</t>
+  </si>
+  <si>
+    <t>Transit Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t>Transit_Mob</t>
+  </si>
+  <si>
+    <t>Workplace Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t>Workplace_Mob</t>
+  </si>
+  <si>
+    <t>Residential Mobility</t>
+  </si>
+  <si>
+    <t>Percent change from baseline for mobility in residences</t>
+  </si>
+  <si>
+    <t>Residential_Mob</t>
+  </si>
+  <si>
+    <t>houseex</t>
+  </si>
+  <si>
+    <t>shapefile</t>
+  </si>
+  <si>
+    <t>change in house hould expenditures from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://www.bps.go.id/indicator/171/533/1/pdrb-adh-konstan-menurut-pengeluaran-2010-100-.html</t>
+  </si>
+  <si>
+    <t>remove commas from data and calculate percent change from raw Q1 and Q2 numbers</t>
+  </si>
+  <si>
+    <t>oil_imports</t>
+  </si>
+  <si>
+    <t>monthly oil and gas imports</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
+  </si>
+  <si>
+    <t>consumex</t>
+  </si>
+  <si>
+    <t>Consumtion Expenditure LNPRT % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>govex</t>
+  </si>
+  <si>
+    <t>Government Consumption Expenditure % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>netex</t>
+  </si>
+  <si>
+    <t>Net Export % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t>GDRP</t>
   </si>
   <si>
     <t xml:space="preserve"> Gross Domestic Regional Expenditure % Change from Q1 to Q2</t>
   </si>
   <si>
-    <t xml:space="preserve">household_ex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household Expenditures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumtion_ex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumtion Expenditure LNPRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gov_ex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government Consumption Expenditure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">net_ex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net Exports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_manu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturing GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_cons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construction GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail and Vehicle Repair GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information and Communication GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health and Social Work GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accomodation and Food Service GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farmer Terms of Trade (have values for each of the 5 provinces)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1y9htQ6XCSQ97M_PmUNJv8V2F0fNSPs5F?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">removed commas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock_index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closing composite stock index (IDX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://drive.google.com/file/d/12brQyMurZj1aQp8jScS5RBKPRe41q-CG/view?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">added in rows for missing dates (weekends and holidays)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">poverty rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://drive.google.com/file/d/1gL2MblktoxtyZoEX1UjuB_B8hVqO4TFT/view?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Querétaro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro</t>
+    <t>household_ex</t>
+  </si>
+  <si>
+    <t>Household Expenditures</t>
+  </si>
+  <si>
+    <t>Consumtion_ex</t>
+  </si>
+  <si>
+    <t>Consumtion Expenditure LNPRT</t>
+  </si>
+  <si>
+    <t>gov_ex</t>
+  </si>
+  <si>
+    <t>Government Consumption Expenditure</t>
+  </si>
+  <si>
+    <t>net_ex</t>
+  </si>
+  <si>
+    <t>Net Exports</t>
+  </si>
+  <si>
+    <t>GDP_manu</t>
+  </si>
+  <si>
+    <t>Manufacturing GDP</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>GDP_cons</t>
+  </si>
+  <si>
+    <t>Construction GDP</t>
+  </si>
+  <si>
+    <t>GDP_retail</t>
+  </si>
+  <si>
+    <t>Retail and Vehicle Repair GDP</t>
+  </si>
+  <si>
+    <t>GDP_IT</t>
+  </si>
+  <si>
+    <t>Information and Communication GDP</t>
+  </si>
+  <si>
+    <t>GDP_social</t>
+  </si>
+  <si>
+    <t>Health and Social Work GDP</t>
+  </si>
+  <si>
+    <t>GDP_food</t>
+  </si>
+  <si>
+    <t>Accomodation and Food Service GDP</t>
+  </si>
+  <si>
+    <t>FTT</t>
+  </si>
+  <si>
+    <t>Farmer Terms of Trade (have values for each of the 5 provinces)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1y9htQ6XCSQ97M_PmUNJv8V2F0fNSPs5F?usp=sharing</t>
+  </si>
+  <si>
+    <t>removed commas</t>
+  </si>
+  <si>
+    <t>stock_index</t>
+  </si>
+  <si>
+    <t>closing composite stock index (IDX</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/12brQyMurZj1aQp8jScS5RBKPRe41q-CG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>added in rows for missing dates (weekends and holidays)</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>poverty rate</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1gL2MblktoxtyZoEX1UjuB_B8hVqO4TFT/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Querétaro</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
   </si>
   <si>
     <r>
@@ -503,186 +507,186 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
+      <t>https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The number of people in hospitals due to coronavirus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assembled from various public announcements, compiled here
+    <t>The number of people in hospitals due to coronavirus.</t>
+  </si>
+  <si>
+    <t>The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
+  </si>
+  <si>
+    <t>The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
+  </si>
+  <si>
+    <t>Assembled from various public announcements, compiled here
 https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
   </si>
   <si>
-    <t xml:space="preserve">Taking dates of policy changes and converting that to daily policy status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average temperature in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of SO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO2 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCNM in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of HCT in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CH4 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of CO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NO in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of NOx in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of O3 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM10 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily average concentration of PM2.5 in the city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro unemployment rate, updated quarterly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RioEmployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil Unemployment Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil unemployment rate, updated monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BraEmployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rain</t>
+    <t>Taking dates of policy changes and converting that to daily policy status</t>
+  </si>
+  <si>
+    <t>Placeholder value</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Daily average temperature in the city</t>
+  </si>
+  <si>
+    <t>https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of SO2 in the city</t>
+  </si>
+  <si>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO2 in the city</t>
+  </si>
+  <si>
+    <t>HCNM</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCNM in the city</t>
+  </si>
+  <si>
+    <t>HCT</t>
+  </si>
+  <si>
+    <t>Daily average concentration of HCT in the city</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CH4 in the city</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of CO in the city</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NO in the city</t>
+  </si>
+  <si>
+    <t>NOx</t>
+  </si>
+  <si>
+    <t>Daily average concentration of NOx in the city</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>Daily average concentration of O3 in the city</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM10 in the city</t>
+  </si>
+  <si>
+    <t>PM2.5</t>
+  </si>
+  <si>
+    <t>Daily average concentration of PM2.5 in the city</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro unemployment rate, updated quarterly</t>
+  </si>
+  <si>
+    <t>RioEmployment</t>
+  </si>
+  <si>
+    <t>Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
+  </si>
+  <si>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Brazil Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Brazil unemployment rate, updated monthly</t>
+  </si>
+  <si>
+    <t>BraEmployment</t>
+  </si>
+  <si>
+    <t>Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
+  </si>
+  <si>
+    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t>Rain</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of rain in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pres</t>
+    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
+  </si>
+  <si>
+    <t>Pres</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of barometric pressure in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">SolRad</t>
+    <t>SolRad</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of solar radiance in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Temp</t>
+    <t>Temp</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of temperature in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Humid</t>
+    <t>Humid</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of relative humidity in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindDir</t>
+    <t>WindDir</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind direction (degrees) in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">WindSpd</t>
+    <t>WindSpd</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind speed in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
@@ -718,29 +722,131 @@
     <t xml:space="preserve">Mean anomaly of PM10 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">PM2_5</t>
+    <t>PM2_5</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of PM2.5 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t xml:space="preserve">Santiago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of the true number of currently infected individuals, as estimated by the ICOVID Chile Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53</t>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>An estimate of the true number of currently infected individuals, as estimated by the ICOVID Chile Group</t>
+  </si>
+  <si>
+    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53</t>
+  </si>
+  <si>
+    <t>DF_chg</t>
+  </si>
+  <si>
+    <t>change in domestic flights from August 2019 to August 2020</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/145s84LbQqBSNG8xhSAKLmbPd69eQh0v9/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compute percent change </t>
+  </si>
+  <si>
+    <t>IF_JK</t>
+  </si>
+  <si>
+    <t>IF_JB</t>
+  </si>
+  <si>
+    <t>IF_JT</t>
+  </si>
+  <si>
+    <t>IF_JI</t>
+  </si>
+  <si>
+    <t>IF_SN</t>
+  </si>
+  <si>
+    <t>DF_JK</t>
+  </si>
+  <si>
+    <t>DF_JI</t>
+  </si>
+  <si>
+    <t>DF_SN</t>
+  </si>
+  <si>
+    <t>Int_F_JK</t>
+  </si>
+  <si>
+    <t>Int_F_JI</t>
+  </si>
+  <si>
+    <t>inflation rate in jakarta</t>
+  </si>
+  <si>
+    <t>inflation rate in west java</t>
+  </si>
+  <si>
+    <t>inflation rate in central java</t>
+  </si>
+  <si>
+    <t>inflation rate in south sulawesi</t>
+  </si>
+  <si>
+    <t>inflation rate in east java</t>
+  </si>
+  <si>
+    <t>IF_Ind_SN</t>
+  </si>
+  <si>
+    <t>IF_Ind_JK</t>
+  </si>
+  <si>
+    <t>IF_Ind_JB</t>
+  </si>
+  <si>
+    <t>IF_Ind_JT</t>
+  </si>
+  <si>
+    <t>IF_Ind_JI</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/11NX_vhnveyy6xB9vfwR4qGmNVh0XZaq4/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>domestic flights jakarta</t>
+  </si>
+  <si>
+    <t>domestic flights east java</t>
+  </si>
+  <si>
+    <t>domestic flights south sulawesi</t>
+  </si>
+  <si>
+    <t>international flights jakarta</t>
+  </si>
+  <si>
+    <t>international flights east java</t>
+  </si>
+  <si>
+    <t>DF_Ind_JK</t>
+  </si>
+  <si>
+    <t>DF_Ind_JI</t>
+  </si>
+  <si>
+    <t>Int_F_Ind_JK</t>
+  </si>
+  <si>
+    <t>Int_F_Ind_JI</t>
+  </si>
+  <si>
+    <t>DF_Ind_SN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -748,22 +854,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -786,7 +877,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -794,101 +885,358 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E96" activeCellId="0" sqref="E96"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="58.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -914,7 +1262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -940,7 +1288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -966,7 +1314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -992,7 +1340,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1018,7 +1366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1044,7 +1392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1070,7 +1418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1096,7 +1444,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
@@ -1122,7 +1470,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1148,7 +1496,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>47</v>
       </c>
@@ -1174,7 +1522,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1198,7 +1546,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1224,11 +1572,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1237,10 +1585,10 @@
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -1250,11 +1598,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1263,10 +1611,10 @@
       <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -1276,7 +1624,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1300,7 +1648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1670,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -1342,7 +1690,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>71</v>
       </c>
@@ -1361,7 +1709,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -1383,7 +1731,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1405,7 +1753,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
@@ -1427,11 +1775,11 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1440,40 +1788,40 @@
       <c r="D23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" t="s">
         <v>70</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="0" t="s">
+      <c r="E24" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>70</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1482,7 +1830,7 @@
       <c r="D25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>77</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1491,11 +1839,11 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1504,18 +1852,18 @@
       <c r="D26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>81</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1524,7 +1872,7 @@
       <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" t="s">
         <v>84</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1533,11 +1881,11 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1546,7 +1894,7 @@
       <c r="D28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>87</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -1555,11 +1903,11 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1568,7 +1916,7 @@
       <c r="D29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>90</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -1577,11 +1925,11 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1590,18 +1938,18 @@
       <c r="D30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" t="s">
         <v>93</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1610,7 +1958,7 @@
       <c r="D31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" t="s">
         <v>96</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -1619,11 +1967,11 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>98</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1645,11 +1993,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1669,11 +2017,11 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>98</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1695,11 +2043,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -1721,11 +2069,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1747,11 +2095,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1773,11 +2121,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -1797,11 +2145,11 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -1820,11 +2168,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1843,11 +2191,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -1867,11 +2215,11 @@
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1890,11 +2238,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -1913,11 +2261,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -1936,11 +2284,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1959,11 +2307,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1982,11 +2330,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -2005,11 +2353,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -2031,11 +2379,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -2057,11 +2405,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>98</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -2083,7 +2431,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
@@ -2107,23 +2455,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="0" t="s">
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" t="s">
         <v>148</v>
       </c>
       <c r="G52" s="5" t="s">
@@ -2133,11 +2481,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -2146,10 +2494,10 @@
       <c r="D53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" t="s">
         <v>148</v>
       </c>
       <c r="G53" s="5" t="s">
@@ -2159,11 +2507,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -2172,10 +2520,10 @@
       <c r="D54" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" t="s">
         <v>148</v>
       </c>
       <c r="G54" s="5" t="s">
@@ -2185,11 +2533,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -2198,10 +2546,10 @@
       <c r="D55" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" t="s">
         <v>148</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -2211,20 +2559,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="0" t="s">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" t="s">
         <v>29</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -2237,11 +2585,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -2250,10 +2598,10 @@
       <c r="D57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" t="s">
         <v>32</v>
       </c>
-      <c r="F57" s="0" t="s">
+      <c r="F57" t="s">
         <v>148</v>
       </c>
       <c r="G57" s="5" t="s">
@@ -2263,7 +2611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>34</v>
       </c>
@@ -2289,11 +2637,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -2305,7 +2653,7 @@
       <c r="E59" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F59" s="0" t="s">
+      <c r="F59" t="s">
         <v>148</v>
       </c>
       <c r="G59" s="5" t="s">
@@ -2315,23 +2663,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="0" t="s">
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
         <v>10</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" t="s">
         <v>45</v>
       </c>
-      <c r="F60" s="0" t="s">
+      <c r="F60" t="s">
         <v>148</v>
       </c>
       <c r="G60" s="5" t="s">
@@ -2341,11 +2689,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -2354,10 +2702,10 @@
       <c r="D61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="0" t="s">
+      <c r="F61" t="s">
         <v>148</v>
       </c>
       <c r="G61" s="5" t="s">
@@ -2367,7 +2715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>51</v>
       </c>
@@ -2393,11 +2741,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -2406,10 +2754,10 @@
       <c r="D63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" t="s">
         <v>58</v>
       </c>
-      <c r="F63" s="0" t="s">
+      <c r="F63" t="s">
         <v>148</v>
       </c>
       <c r="G63" s="1" t="s">
@@ -2419,11 +2767,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -2432,10 +2780,10 @@
       <c r="D64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" t="s">
         <v>158</v>
       </c>
-      <c r="F64" s="0" t="s">
+      <c r="F64" t="s">
         <v>148</v>
       </c>
       <c r="G64" s="5" t="s">
@@ -2445,11 +2793,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>162</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -2458,10 +2806,10 @@
       <c r="D65" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" t="s">
         <v>162</v>
       </c>
-      <c r="F65" s="0" t="s">
+      <c r="F65" t="s">
         <v>148</v>
       </c>
       <c r="G65" s="5" t="s">
@@ -2471,11 +2819,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>165</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -2484,10 +2832,10 @@
       <c r="D66" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" t="s">
         <v>165</v>
       </c>
-      <c r="F66" s="0" t="s">
+      <c r="F66" t="s">
         <v>148</v>
       </c>
       <c r="G66" s="5" t="s">
@@ -2497,11 +2845,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>167</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>9</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -2510,10 +2858,10 @@
       <c r="D67" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" t="s">
         <v>167</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F67" t="s">
         <v>148</v>
       </c>
       <c r="G67" s="5" t="s">
@@ -2523,11 +2871,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>169</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -2536,10 +2884,10 @@
       <c r="D68" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" t="s">
         <v>169</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="F68" t="s">
         <v>148</v>
       </c>
       <c r="G68" s="5" t="s">
@@ -2549,11 +2897,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>171</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -2562,10 +2910,10 @@
       <c r="D69" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" t="s">
         <v>171</v>
       </c>
-      <c r="F69" s="0" t="s">
+      <c r="F69" t="s">
         <v>148</v>
       </c>
       <c r="G69" s="5" t="s">
@@ -2575,11 +2923,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>173</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="4" t="s">
@@ -2588,10 +2936,10 @@
       <c r="D70" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" t="s">
         <v>173</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" t="s">
         <v>148</v>
       </c>
       <c r="G70" s="5" t="s">
@@ -2601,11 +2949,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>9</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -2614,10 +2962,10 @@
       <c r="D71" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" t="s">
         <v>175</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="F71" t="s">
         <v>148</v>
       </c>
       <c r="G71" s="5" t="s">
@@ -2627,11 +2975,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>177</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -2640,10 +2988,10 @@
       <c r="D72" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" t="s">
         <v>177</v>
       </c>
-      <c r="F72" s="0" t="s">
+      <c r="F72" t="s">
         <v>148</v>
       </c>
       <c r="G72" s="5" t="s">
@@ -2653,11 +3001,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>179</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -2666,10 +3014,10 @@
       <c r="D73" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" t="s">
         <v>179</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" t="s">
         <v>148</v>
       </c>
       <c r="G73" s="5" t="s">
@@ -2679,11 +3027,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>181</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -2692,10 +3040,10 @@
       <c r="D74" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" t="s">
         <v>181</v>
       </c>
-      <c r="F74" s="0" t="s">
+      <c r="F74" t="s">
         <v>148</v>
       </c>
       <c r="G74" s="5" t="s">
@@ -2705,11 +3053,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>183</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="4" t="s">
@@ -2718,10 +3066,10 @@
       <c r="D75" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" t="s">
         <v>183</v>
       </c>
-      <c r="F75" s="0" t="s">
+      <c r="F75" t="s">
         <v>148</v>
       </c>
       <c r="G75" s="5" t="s">
@@ -2731,11 +3079,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>185</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -2744,10 +3092,10 @@
       <c r="D76" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" t="s">
         <v>187</v>
       </c>
-      <c r="F76" s="0" t="s">
+      <c r="F76" t="s">
         <v>148</v>
       </c>
       <c r="G76" s="5" t="s">
@@ -2757,11 +3105,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>190</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -2770,10 +3118,10 @@
       <c r="D77" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" t="s">
         <v>192</v>
       </c>
-      <c r="F77" s="0" t="s">
+      <c r="F77" t="s">
         <v>148</v>
       </c>
       <c r="G77" s="1" t="s">
@@ -2783,11 +3131,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>195</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>98</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -2796,10 +3144,10 @@
       <c r="D78" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" t="s">
         <v>157</v>
       </c>
-      <c r="F78" s="0" t="s">
+      <c r="F78" t="s">
         <v>148</v>
       </c>
       <c r="G78" s="5" t="s">
@@ -2809,11 +3157,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>198</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>98</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -2822,10 +3170,10 @@
       <c r="D79" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" t="s">
         <v>157</v>
       </c>
-      <c r="F79" s="0" t="s">
+      <c r="F79" t="s">
         <v>148</v>
       </c>
       <c r="G79" s="5" t="s">
@@ -2835,11 +3183,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>200</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>98</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -2848,10 +3196,10 @@
       <c r="D80" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E80" s="0" t="s">
+      <c r="E80" t="s">
         <v>157</v>
       </c>
-      <c r="F80" s="0" t="s">
+      <c r="F80" t="s">
         <v>148</v>
       </c>
       <c r="G80" s="5" t="s">
@@ -2861,11 +3209,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>202</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>98</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -2874,10 +3222,10 @@
       <c r="D81" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" t="s">
         <v>157</v>
       </c>
-      <c r="F81" s="0" t="s">
+      <c r="F81" t="s">
         <v>148</v>
       </c>
       <c r="G81" s="5" t="s">
@@ -2887,11 +3235,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" t="s">
         <v>98</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -2900,10 +3248,10 @@
       <c r="D82" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E82" s="0" t="s">
+      <c r="E82" t="s">
         <v>157</v>
       </c>
-      <c r="F82" s="0" t="s">
+      <c r="F82" t="s">
         <v>148</v>
       </c>
       <c r="G82" s="5" t="s">
@@ -2913,11 +3261,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>206</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" t="s">
         <v>98</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2926,10 +3274,10 @@
       <c r="D83" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E83" s="0" t="s">
+      <c r="E83" t="s">
         <v>157</v>
       </c>
-      <c r="F83" s="0" t="s">
+      <c r="F83" t="s">
         <v>148</v>
       </c>
       <c r="G83" s="5" t="s">
@@ -2939,11 +3287,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>208</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="4" t="s">
@@ -2952,10 +3300,10 @@
       <c r="D84" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E84" s="0" t="s">
+      <c r="E84" t="s">
         <v>157</v>
       </c>
-      <c r="F84" s="0" t="s">
+      <c r="F84" t="s">
         <v>148</v>
       </c>
       <c r="G84" s="5" t="s">
@@ -2965,11 +3313,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+    <row r="85" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>162</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" t="s">
         <v>98</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -2978,10 +3326,10 @@
       <c r="D85" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E85" s="0" t="s">
+      <c r="E85" t="s">
         <v>157</v>
       </c>
-      <c r="F85" s="0" t="s">
+      <c r="F85" t="s">
         <v>148</v>
       </c>
       <c r="G85" s="5" t="s">
@@ -2991,11 +3339,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>165</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" t="s">
         <v>98</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -3004,10 +3352,10 @@
       <c r="D86" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E86" s="0" t="s">
+      <c r="E86" t="s">
         <v>157</v>
       </c>
-      <c r="F86" s="0" t="s">
+      <c r="F86" t="s">
         <v>148</v>
       </c>
       <c r="G86" s="5" t="s">
@@ -3017,11 +3365,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="87" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>167</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" t="s">
         <v>98</v>
       </c>
       <c r="C87" s="4" t="s">
@@ -3030,10 +3378,10 @@
       <c r="D87" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E87" s="0" t="s">
+      <c r="E87" t="s">
         <v>157</v>
       </c>
-      <c r="F87" s="0" t="s">
+      <c r="F87" t="s">
         <v>148</v>
       </c>
       <c r="G87" s="5" t="s">
@@ -3043,11 +3391,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" t="s">
         <v>98</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -3056,10 +3404,10 @@
       <c r="D88" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E88" s="0" t="s">
+      <c r="E88" t="s">
         <v>157</v>
       </c>
-      <c r="F88" s="0" t="s">
+      <c r="F88" t="s">
         <v>148</v>
       </c>
       <c r="G88" s="5" t="s">
@@ -3069,11 +3417,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>171</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" t="s">
         <v>98</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -3082,10 +3430,10 @@
       <c r="D89" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E89" s="0" t="s">
+      <c r="E89" t="s">
         <v>157</v>
       </c>
-      <c r="F89" s="0" t="s">
+      <c r="F89" t="s">
         <v>148</v>
       </c>
       <c r="G89" s="5" t="s">
@@ -3095,11 +3443,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+    <row r="90" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>173</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" t="s">
         <v>98</v>
       </c>
       <c r="C90" s="4" t="s">
@@ -3108,10 +3456,10 @@
       <c r="D90" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E90" s="0" t="s">
+      <c r="E90" t="s">
         <v>157</v>
       </c>
-      <c r="F90" s="0" t="s">
+      <c r="F90" t="s">
         <v>148</v>
       </c>
       <c r="G90" s="5" t="s">
@@ -3121,11 +3469,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="91" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>175</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" t="s">
         <v>98</v>
       </c>
       <c r="C91" s="4" t="s">
@@ -3134,10 +3482,10 @@
       <c r="D91" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E91" s="0" t="s">
+      <c r="E91" t="s">
         <v>157</v>
       </c>
-      <c r="F91" s="0" t="s">
+      <c r="F91" t="s">
         <v>148</v>
       </c>
       <c r="G91" s="5" t="s">
@@ -3147,11 +3495,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="92" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>177</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" t="s">
         <v>98</v>
       </c>
       <c r="C92" s="4" t="s">
@@ -3160,10 +3508,10 @@
       <c r="D92" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E92" s="0" t="s">
+      <c r="E92" t="s">
         <v>157</v>
       </c>
-      <c r="F92" s="0" t="s">
+      <c r="F92" t="s">
         <v>148</v>
       </c>
       <c r="G92" s="5" t="s">
@@ -3173,11 +3521,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+    <row r="93" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>179</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" t="s">
         <v>98</v>
       </c>
       <c r="C93" s="4" t="s">
@@ -3186,10 +3534,10 @@
       <c r="D93" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E93" s="0" t="s">
+      <c r="E93" t="s">
         <v>157</v>
       </c>
-      <c r="F93" s="0" t="s">
+      <c r="F93" t="s">
         <v>148</v>
       </c>
       <c r="G93" s="5" t="s">
@@ -3199,11 +3547,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="94" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>181</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" t="s">
         <v>98</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -3212,10 +3560,10 @@
       <c r="D94" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E94" s="0" t="s">
+      <c r="E94" t="s">
         <v>157</v>
       </c>
-      <c r="F94" s="0" t="s">
+      <c r="F94" t="s">
         <v>148</v>
       </c>
       <c r="G94" s="5" t="s">
@@ -3225,11 +3573,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+    <row r="95" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>220</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" t="s">
         <v>98</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -3238,10 +3586,10 @@
       <c r="D95" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E95" s="0" t="s">
+      <c r="E95" t="s">
         <v>157</v>
       </c>
-      <c r="F95" s="0" t="s">
+      <c r="F95" t="s">
         <v>148</v>
       </c>
       <c r="G95" s="5" t="s">
@@ -3251,7 +3599,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>8</v>
       </c>
@@ -3277,7 +3625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>24</v>
       </c>
@@ -3303,7 +3651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>71</v>
       </c>
@@ -3329,7 +3677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>34</v>
       </c>
@@ -3355,7 +3703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>39</v>
       </c>
@@ -3381,7 +3729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>43</v>
       </c>
@@ -3407,7 +3755,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>51</v>
       </c>
@@ -3431,62 +3779,316 @@
         <v>55</v>
       </c>
     </row>
+    <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>229</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E104" t="s">
+        <v>245</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>230</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E105" t="s">
+        <v>246</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>231</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E106" t="s">
+        <v>247</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>232</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E107" t="s">
+        <v>244</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>233</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E108" t="s">
+        <v>248</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>234</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E109" t="s">
+        <v>255</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>235</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E110" t="s">
+        <v>256</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>236</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E111" t="s">
+        <v>259</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>237</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E112" t="s">
+        <v>257</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E113" t="s">
+        <v>258</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H102"/>
+  <autoFilter ref="A1:H102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8"/>
-    <hyperlink ref="G4" r:id="rId3" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G6" r:id="rId4" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G7" r:id="rId5" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G9" r:id="rId6" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G10" r:id="rId7" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
-    <hyperlink ref="G11" r:id="rId8" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8"/>
-    <hyperlink ref="G13" r:id="rId9" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20"/>
-    <hyperlink ref="G14" r:id="rId10" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7"/>
-    <hyperlink ref="G15" r:id="rId11" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40"/>
-    <hyperlink ref="G62" r:id="rId12" display="Assembled from various public announcements, compiled here&#10;https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing"/>
-    <hyperlink ref="G64" r:id="rId13" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G65" r:id="rId14" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G66" r:id="rId15" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G67" r:id="rId16" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G68" r:id="rId17" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G69" r:id="rId18" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G70" r:id="rId19" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G71" r:id="rId20" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G72" r:id="rId21" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G73" r:id="rId22" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G74" r:id="rId23" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G75" r:id="rId24" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G76" r:id="rId25" display="Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados"/>
-    <hyperlink ref="G78" r:id="rId26" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G79" r:id="rId27" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G80" r:id="rId28" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G81" r:id="rId29" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G82" r:id="rId30" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G83" r:id="rId31" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G84" r:id="rId32" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G85" r:id="rId33" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G86" r:id="rId34" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G87" r:id="rId35" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G88" r:id="rId36" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G89" r:id="rId37" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G90" r:id="rId38" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G91" r:id="rId39" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G92" r:id="rId40" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G93" r:id="rId41" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G94" r:id="rId42" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G95" r:id="rId43" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
-    <hyperlink ref="G98" r:id="rId44" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53"/>
-    <hyperlink ref="G101" r:id="rId45" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G62" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G64" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G65" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G66" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G67" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G68" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G69" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G70" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G71" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G72" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G73" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G74" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G75" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G76" r:id="rId25" display="Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G78" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G79" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G80" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G81" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G82" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G83" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G84" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G85" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G86" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G87" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G88" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G89" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G90" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="G91" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G92" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="G93" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G94" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="G95" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="G98" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="G101" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId46"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding foreign visitor and hotel occupancy data to Indonesia
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944D8965-BFFD-49DB-8D6F-4257D5D1A174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9408CA8-E7F2-48D9-B3C0-D15019EB75E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="279">
   <si>
     <t>Header or Field Name</t>
   </si>
@@ -840,6 +840,63 @@
   </si>
   <si>
     <t>DF_Ind_SN</t>
+  </si>
+  <si>
+    <t>foreign</t>
+  </si>
+  <si>
+    <t>HO_JK</t>
+  </si>
+  <si>
+    <t>HO_JB</t>
+  </si>
+  <si>
+    <t>HO_JT</t>
+  </si>
+  <si>
+    <t>HO_JI</t>
+  </si>
+  <si>
+    <t>HO_SN</t>
+  </si>
+  <si>
+    <t>foreign visitors</t>
+  </si>
+  <si>
+    <t>hotel occupancy Jakarta</t>
+  </si>
+  <si>
+    <t>hotel occupancy west java</t>
+  </si>
+  <si>
+    <t>hotel occupancy central java</t>
+  </si>
+  <si>
+    <t>hotel occupancy east java</t>
+  </si>
+  <si>
+    <t>HO_Ind_JK</t>
+  </si>
+  <si>
+    <t>HO_Ind_JB</t>
+  </si>
+  <si>
+    <t>HO_Ind_JT</t>
+  </si>
+  <si>
+    <t>HO_Ind_JI</t>
+  </si>
+  <si>
+    <t>HO_Ind_SN</t>
+  </si>
+  <si>
+    <t>hotel occupancy south sulawesi</t>
+  </si>
+  <si>
+    <t>foreign_vis_Ind</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1g9OeNpLuXKhCqu7EqZSfP5XLvWBKquhr/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -1218,11 +1275,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3805,7 +3862,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>229</v>
       </c>
@@ -4033,6 +4090,141 @@
       </c>
       <c r="G113" s="1" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>260</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E114" t="s">
+        <v>277</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>261</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E115" t="s">
+        <v>271</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>262</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E116" t="s">
+        <v>272</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>263</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E117" t="s">
+        <v>273</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>264</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E118" t="s">
+        <v>274</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>265</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E119" t="s">
+        <v>275</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating vida and adding a bunch of nightlights related graphs
</commit_message>
<xml_diff>
--- a/Data/Data_Descriptions.xlsx
+++ b/Data/Data_Descriptions.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9408CA8-E7F2-48D9-B3C0-D15019EB75E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$H$99</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$99</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -30,452 +26,452 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="279">
   <si>
-    <t>Header or Field Name</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Related SD Objects</t>
-  </si>
-  <si>
-    <t>Context Area</t>
-  </si>
-  <si>
-    <t>Data Source</t>
-  </si>
-  <si>
-    <t>Required Processing</t>
-  </si>
-  <si>
-    <t>Susceptible Population</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>Commonly Used SEIR Data</t>
-  </si>
-  <si>
-    <t>Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
-  </si>
-  <si>
-    <t>SPop</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv</t>
-  </si>
-  <si>
-    <t>Basic arithmetic from raw data</t>
-  </si>
-  <si>
-    <t>Hospitalized Population</t>
+    <t xml:space="preserve">Header or Field Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related SD Objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susceptible Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commonly Used SEIR Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since there is no current characterization of what proportion of the population is immune to coronavirus, this is defined as the total population of the context area minus those infected (hospitalized and not), recovered, and dead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic from raw data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitalized Population</t>
   </si>
   <si>
     <t xml:space="preserve">The number of people in hospital Intensive Care Units (ICU) due to coronavirus. </t>
   </si>
   <si>
-    <t>Hpop</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Recovered Population</t>
-  </si>
-  <si>
-    <t>The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
-  </si>
-  <si>
-    <t>Rpop</t>
-  </si>
-  <si>
-    <t>Measured Current Infected</t>
-  </si>
-  <si>
-    <t>The number of active cases, as defined by the Ministry of Health</t>
-  </si>
-  <si>
-    <t>mTotIPop</t>
-  </si>
-  <si>
-    <t>Measured Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t>The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
-  </si>
-  <si>
-    <t>mIPop</t>
-  </si>
-  <si>
-    <t>True Unhospitalized Infected</t>
-  </si>
-  <si>
-    <t>An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
-  </si>
-  <si>
-    <t>IPop</t>
-  </si>
-  <si>
-    <t>Placeholder: Samples from a normal distribution that ses the Measured Unhospitalized Infected from one week in the future as the mean and 0.25*that value as the standard deviation
+    <t xml:space="preserve">Hpop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recovered Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as calculated from the measured current infected, hospital departures, and deaths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rpop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of active cases, as defined by the Ministry of Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mTotIPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have been individually, positively identified as currently having coronavirus but not currently hospitalized. Calculated from Measured Current Infected and Hospitalized Population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mIPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Unhospitalized Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An estimate of the true number of unhospitalized, currently infected individuals, which is likely higher than the measured cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder: Samples from a normal distribution that ses the Measured Unhospitalized Infected from one week in the future as the mean and 0.25*that value as the standard deviation
 NORMINV(RAND(),Measured Unhospitalized Infected (1 week in future),0.25*Measured Unhospitalized Infected (1 week in future))</t>
   </si>
   <si>
-    <t>Accumulative Deaths</t>
-  </si>
-  <si>
-    <t>Accumulative deaths attributed to coronavirus.</t>
-  </si>
-  <si>
-    <t>Deaths</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto14</t>
-  </si>
-  <si>
-    <t>Sum across regions</t>
-  </si>
-  <si>
-    <t>Measured Infection Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of infection, based on Measured Current Infected</t>
-  </si>
-  <si>
-    <t>mInfectR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
-  </si>
-  <si>
-    <t>True Infection Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of infection, based on True Current Infected</t>
-  </si>
-  <si>
-    <t>InfectR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of True Current Infected</t>
-  </si>
-  <si>
-    <t>Hospitalization Rate</t>
-  </si>
-  <si>
-    <t>Daily rate of hospitalization, based on Hospitalized Population</t>
-  </si>
-  <si>
-    <t>HosR</t>
-  </si>
-  <si>
-    <t>Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
-  </si>
-  <si>
-    <t>Closure Policy</t>
-  </si>
-  <si>
-    <t>Policy and Equipment Data</t>
-  </si>
-  <si>
-    <t>Chile’s closure policy status, as defined by the Paso a Paso program</t>
-  </si>
-  <si>
-    <t>ClosureP</t>
-  </si>
-  <si>
-    <t>Placeholder: need to identify actual history, varies from province to province</t>
-  </si>
-  <si>
-    <t>Ventilators</t>
-  </si>
-  <si>
-    <t>Number of available ventilators</t>
-  </si>
-  <si>
-    <t>Vents</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20</t>
-  </si>
-  <si>
-    <t>PCR Tests</t>
-  </si>
-  <si>
-    <t>Daily number of PCR tests for coronavirus conducted</t>
-  </si>
-  <si>
-    <t>PCR</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7</t>
-  </si>
-  <si>
-    <t>Air Passengers</t>
-  </si>
-  <si>
-    <t>Socioeconomic Data</t>
-  </si>
-  <si>
-    <t>Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
-  </si>
-  <si>
-    <t>AirPass</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40</t>
-  </si>
-  <si>
-    <t>Sum across destination regions</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>True Current Infected</t>
-  </si>
-  <si>
-    <t>Currently a placeholder</t>
-  </si>
-  <si>
-    <t>Gross Domestic Product</t>
-  </si>
-  <si>
-    <t>GDP_Ind</t>
-  </si>
-  <si>
-    <t>Arrivals</t>
-  </si>
-  <si>
-    <t>Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
-  </si>
-  <si>
-    <t>Arrivals_Ind</t>
-  </si>
-  <si>
-    <t>Retail and Recreation Mobility</t>
-  </si>
-  <si>
-    <t>Environmental Data</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in retail and recreation</t>
-  </si>
-  <si>
-    <t>Retail_Mob</t>
-  </si>
-  <si>
-    <t>Grocery and Pharmacy Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in Grocery and Pharmacy</t>
-  </si>
-  <si>
-    <t>Grocery_Mob</t>
-  </si>
-  <si>
-    <t>Parks Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in parks</t>
-  </si>
-  <si>
-    <t>Parks_Mob</t>
-  </si>
-  <si>
-    <t>Transit Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility for transit</t>
-  </si>
-  <si>
-    <t>Transit_Mob</t>
-  </si>
-  <si>
-    <t>Workplace Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in workplaces</t>
-  </si>
-  <si>
-    <t>Workplace_Mob</t>
-  </si>
-  <si>
-    <t>Residential Mobility</t>
-  </si>
-  <si>
-    <t>Percent change from baseline for mobility in residences</t>
-  </si>
-  <si>
-    <t>Residential_Mob</t>
-  </si>
-  <si>
-    <t>houseex</t>
-  </si>
-  <si>
-    <t>shapefile</t>
-  </si>
-  <si>
-    <t>change in house hould expenditures from Q1 to Q2</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>https://www.bps.go.id/indicator/171/533/1/pdrb-adh-konstan-menurut-pengeluaran-2010-100-.html</t>
-  </si>
-  <si>
-    <t>remove commas from data and calculate percent change from raw Q1 and Q2 numbers</t>
-  </si>
-  <si>
-    <t>oil_imports</t>
-  </si>
-  <si>
-    <t>monthly oil and gas imports</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
-  </si>
-  <si>
-    <t>consumex</t>
-  </si>
-  <si>
-    <t>Consumtion Expenditure LNPRT % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t>govex</t>
-  </si>
-  <si>
-    <t>Government Consumption Expenditure % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t>netex</t>
-  </si>
-  <si>
-    <t>Net Export % Change from Q1 to Q2</t>
-  </si>
-  <si>
-    <t>GDRP</t>
+    <t xml:space="preserve">Accumulative Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accumulative deaths attributed to coronavirus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum across regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured Infection Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of infection, based on Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mInfectR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Measured Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Infection Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of infection, based on True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InfectR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitalization Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of hospitalization, based on Hospitalized Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HosR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic arithmetic, just current day minus previous day of Hospitalized Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closure Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy and Equipment Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile’s closure policy status, as defined by the Paso a Paso program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClosureP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder: need to identify actual history, varies from province to province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of available ventilators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCR Tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily number of PCR tests for coronavirus conducted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Passengers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socioeconomic Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of air travel passengers arriving in Chile, originating either inside or outside of Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AirPass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum across destination regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Current Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently a placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_Ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrivals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of visitor arrivals per month in Indonesia. Available data ends in June, so post-June values are a placeholder for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrivals_Ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail and Recreation Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in retail and recreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery and Pharmacy Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in Grocery and Pharmacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parks Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in parks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parks_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility for transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workplace Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in workplaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workplace_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change from baseline for mobility in residences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential_Mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">houseex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shapefile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change in house hould expenditures from Q1 to Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bps.go.id/indicator/171/533/1/pdrb-adh-konstan-menurut-pengeluaran-2010-100-.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove commas from data and calculate percent change from raw Q1 and Q2 numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oil_imports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthly oil and gas imports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1gg1jPYMPD0pWS5mMMmnUMTnYY39pWnFI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumtion Expenditure LNPRT % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">govex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Consumption Expenditure % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Export % Change from Q1 to Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDRP</t>
   </si>
   <si>
     <t xml:space="preserve"> Gross Domestic Regional Expenditure % Change from Q1 to Q2</t>
   </si>
   <si>
-    <t>household_ex</t>
-  </si>
-  <si>
-    <t>Household Expenditures</t>
-  </si>
-  <si>
-    <t>Consumtion_ex</t>
-  </si>
-  <si>
-    <t>Consumtion Expenditure LNPRT</t>
-  </si>
-  <si>
-    <t>gov_ex</t>
-  </si>
-  <si>
-    <t>Government Consumption Expenditure</t>
-  </si>
-  <si>
-    <t>net_ex</t>
-  </si>
-  <si>
-    <t>Net Exports</t>
-  </si>
-  <si>
-    <t>GDP_manu</t>
-  </si>
-  <si>
-    <t>Manufacturing GDP</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>GDP_cons</t>
-  </si>
-  <si>
-    <t>Construction GDP</t>
-  </si>
-  <si>
-    <t>GDP_retail</t>
-  </si>
-  <si>
-    <t>Retail and Vehicle Repair GDP</t>
-  </si>
-  <si>
-    <t>GDP_IT</t>
-  </si>
-  <si>
-    <t>Information and Communication GDP</t>
-  </si>
-  <si>
-    <t>GDP_social</t>
-  </si>
-  <si>
-    <t>Health and Social Work GDP</t>
-  </si>
-  <si>
-    <t>GDP_food</t>
-  </si>
-  <si>
-    <t>Accomodation and Food Service GDP</t>
-  </si>
-  <si>
-    <t>FTT</t>
-  </si>
-  <si>
-    <t>Farmer Terms of Trade (have values for each of the 5 provinces)</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1y9htQ6XCSQ97M_PmUNJv8V2F0fNSPs5F?usp=sharing</t>
-  </si>
-  <si>
-    <t>removed commas</t>
-  </si>
-  <si>
-    <t>stock_index</t>
-  </si>
-  <si>
-    <t>closing composite stock index (IDX</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/12brQyMurZj1aQp8jScS5RBKPRe41q-CG/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>added in rows for missing dates (weekends and holidays)</t>
-  </si>
-  <si>
-    <t>pov</t>
-  </si>
-  <si>
-    <t>poverty rate</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1gL2MblktoxtyZoEX1UjuB_B8hVqO4TFT/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Querétaro</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro</t>
+    <t xml:space="preserve">household_ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Expenditures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumtion_ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumtion Expenditure LNPRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Consumption Expenditure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net_ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Exports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_manu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1ZFOUjbSuxiCDNyCk08YMa5s0tSvXjEWP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_cons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_retail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail and Vehicle Repair GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information and Communication GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health and Social Work GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP_food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accomodation and Food Service GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmer Terms of Trade (have values for each of the 5 provinces)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1y9htQ6XCSQ97M_PmUNJv8V2F0fNSPs5F?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed commas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closing composite stock index (IDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/12brQyMurZj1aQp8jScS5RBKPRe41q-CG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added in rows for missing dates (weekends and holidays)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poverty rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1gL2MblktoxtyZoEX1UjuB_B8hVqO4TFT/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Querétaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro</t>
   </si>
   <si>
     <r>
@@ -507,186 +503,186 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
+      <t xml:space="preserve">https://www.data.rio/datasets/dados-individuais-dos-casos-confirmados-de-covid-19-no-munic%C3%ADpio-do-rio-de-janeiro-2</t>
     </r>
   </si>
   <si>
-    <t>The number of people in hospitals due to coronavirus.</t>
-  </si>
-  <si>
-    <t>The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
-  </si>
-  <si>
-    <t>The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
-  </si>
-  <si>
-    <t>Assembled from various public announcements, compiled here
+    <t xml:space="preserve">The number of people in hospitals due to coronavirus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of people who have recovered from coronavirus cases, as defined by Rio de Janeiro health officials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current number of people who have been individually, positively identified as currently having coronavirus. Calculated from the accumulative case count, the recovered population, and deaths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro’s closure policy status, as defined by the 6 Fases program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assembled from various public announcements, compiled here
 https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing</t>
   </si>
   <si>
-    <t>Taking dates of policy changes and converting that to daily policy status</t>
-  </si>
-  <si>
-    <t>Placeholder value</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Daily average temperature in the city</t>
-  </si>
-  <si>
-    <t>https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
-  </si>
-  <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
-  </si>
-  <si>
-    <t>SO2</t>
-  </si>
-  <si>
-    <t>Daily average concentration of SO2 in the city</t>
-  </si>
-  <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
-  </si>
-  <si>
-    <t>NO2</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NO2 in the city</t>
-  </si>
-  <si>
-    <t>HCNM</t>
-  </si>
-  <si>
-    <t>Daily average concentration of HCNM in the city</t>
-  </si>
-  <si>
-    <t>HCT</t>
-  </si>
-  <si>
-    <t>Daily average concentration of HCT in the city</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>Daily average concentration of CH4 in the city</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>Daily average concentration of CO in the city</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NO in the city</t>
-  </si>
-  <si>
-    <t>NOx</t>
-  </si>
-  <si>
-    <t>Daily average concentration of NOx in the city</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>Daily average concentration of O3 in the city</t>
-  </si>
-  <si>
-    <t>PM10</t>
-  </si>
-  <si>
-    <t>Daily average concentration of PM10 in the city</t>
-  </si>
-  <si>
-    <t>PM2.5</t>
-  </si>
-  <si>
-    <t>Daily average concentration of PM2.5 in the city</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro Unemployment Rate</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro unemployment rate, updated quarterly</t>
-  </si>
-  <si>
-    <t>RioEmployment</t>
-  </si>
-  <si>
-    <t>Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
-  </si>
-  <si>
-    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t>Brazil Unemployment Rate</t>
-  </si>
-  <si>
-    <t>Brazil unemployment rate, updated monthly</t>
-  </si>
-  <si>
-    <t>BraEmployment</t>
-  </si>
-  <si>
-    <t>Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
-  </si>
-  <si>
-    <t>Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
-  </si>
-  <si>
-    <t>Rain</t>
+    <t xml:space="preserve">Taking dates of policy changes and converting that to daily policy status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average temperature in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of SO2 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NO2 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCNM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of HCNM in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of HCT in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of CH4 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of CO in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NO in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of NOx in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of O3 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of PM10 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily average concentration of PM2.5 in the city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro unemployment rate, updated quarterly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RioEmployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from trimester to daily data, convert employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil unemployment rate, updated monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BraEmployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly Disclosure Data available here: https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9171-pesquisa-nacional-por-amostra-de-domicilios-continua-mensal.html?=&amp;t=o-que-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have to pull out the relevant data from multi-sheet spreadsheet, convert from monthly to daily data, convert from employment rate to unemployment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rain</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of rain in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
-  </si>
-  <si>
-    <t>Pres</t>
+    <t xml:space="preserve">Using a Python script to convert hourly data for each location and calculate daily average for entire city, then calculate mean anomaly for the given reference and observation periods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pres</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of barometric pressure in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>SolRad</t>
+    <t xml:space="preserve">SolRad</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of solar radiance in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Temp</t>
+    <t xml:space="preserve">Temp</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of temperature in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Humid</t>
+    <t xml:space="preserve">Humid</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of relative humidity in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>WindDir</t>
+    <t xml:space="preserve">WindDir</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind direction (degrees) in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>WindSpd</t>
+    <t xml:space="preserve">WindSpd</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of wind speed in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
@@ -722,188 +718,191 @@
     <t xml:space="preserve">Mean anomaly of PM10 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>PM2_5</t>
+    <t xml:space="preserve">PM2_5</t>
   </si>
   <si>
     <t xml:space="preserve">Mean anomaly of PM2.5 in Rio de Janeiro using a reference period of 01/Jan/2011 – 15/Feb/2020 and an observation period of 16/Feb/2020 – Present. </t>
   </si>
   <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>An estimate of the true number of currently infected individuals, as estimated by the ICOVID Chile Group</t>
-  </si>
-  <si>
-    <t>https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53</t>
-  </si>
-  <si>
-    <t>DF_chg</t>
-  </si>
-  <si>
-    <t>change in domestic flights from August 2019 to August 2020</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/145s84LbQqBSNG8xhSAKLmbPd69eQh0v9/view?usp=sharing</t>
+    <t xml:space="preserve">Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An estimate of the true number of currently infected individuals, as estimated by the ICOVID Chile Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_chg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change in domestic flights from August 2019 to August 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/145s84LbQqBSNG8xhSAKLmbPd69eQh0v9/view?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">compute percent change </t>
   </si>
   <si>
-    <t>IF_JK</t>
-  </si>
-  <si>
-    <t>IF_JB</t>
-  </si>
-  <si>
-    <t>IF_JT</t>
-  </si>
-  <si>
-    <t>IF_JI</t>
-  </si>
-  <si>
-    <t>IF_SN</t>
-  </si>
-  <si>
-    <t>DF_JK</t>
-  </si>
-  <si>
-    <t>DF_JI</t>
-  </si>
-  <si>
-    <t>DF_SN</t>
-  </si>
-  <si>
-    <t>Int_F_JK</t>
-  </si>
-  <si>
-    <t>Int_F_JI</t>
-  </si>
-  <si>
-    <t>inflation rate in jakarta</t>
-  </si>
-  <si>
-    <t>inflation rate in west java</t>
-  </si>
-  <si>
-    <t>inflation rate in central java</t>
-  </si>
-  <si>
-    <t>inflation rate in south sulawesi</t>
-  </si>
-  <si>
-    <t>inflation rate in east java</t>
-  </si>
-  <si>
-    <t>IF_Ind_SN</t>
-  </si>
-  <si>
-    <t>IF_Ind_JK</t>
-  </si>
-  <si>
-    <t>IF_Ind_JB</t>
-  </si>
-  <si>
-    <t>IF_Ind_JT</t>
-  </si>
-  <si>
-    <t>IF_Ind_JI</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/11NX_vhnveyy6xB9vfwR4qGmNVh0XZaq4/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>domestic flights jakarta</t>
-  </si>
-  <si>
-    <t>domestic flights east java</t>
-  </si>
-  <si>
-    <t>domestic flights south sulawesi</t>
-  </si>
-  <si>
-    <t>international flights jakarta</t>
-  </si>
-  <si>
-    <t>international flights east java</t>
-  </si>
-  <si>
-    <t>DF_Ind_JK</t>
-  </si>
-  <si>
-    <t>DF_Ind_JI</t>
-  </si>
-  <si>
-    <t>Int_F_Ind_JK</t>
-  </si>
-  <si>
-    <t>Int_F_Ind_JI</t>
-  </si>
-  <si>
-    <t>DF_Ind_SN</t>
-  </si>
-  <si>
-    <t>foreign</t>
-  </si>
-  <si>
-    <t>HO_JK</t>
-  </si>
-  <si>
-    <t>HO_JB</t>
-  </si>
-  <si>
-    <t>HO_JT</t>
-  </si>
-  <si>
-    <t>HO_JI</t>
-  </si>
-  <si>
-    <t>HO_SN</t>
-  </si>
-  <si>
-    <t>foreign visitors</t>
-  </si>
-  <si>
-    <t>hotel occupancy Jakarta</t>
-  </si>
-  <si>
-    <t>hotel occupancy west java</t>
-  </si>
-  <si>
-    <t>hotel occupancy central java</t>
-  </si>
-  <si>
-    <t>hotel occupancy east java</t>
-  </si>
-  <si>
-    <t>HO_Ind_JK</t>
-  </si>
-  <si>
-    <t>HO_Ind_JB</t>
-  </si>
-  <si>
-    <t>HO_Ind_JT</t>
-  </si>
-  <si>
-    <t>HO_Ind_JI</t>
-  </si>
-  <si>
-    <t>HO_Ind_SN</t>
-  </si>
-  <si>
-    <t>hotel occupancy south sulawesi</t>
-  </si>
-  <si>
-    <t>foreign_vis_Ind</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1g9OeNpLuXKhCqu7EqZSfP5XLvWBKquhr/view?usp=sharing</t>
+    <t xml:space="preserve">IF_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation rate in jakarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_Ind_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/11NX_vhnveyy6xB9vfwR4qGmNVh0XZaq4/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation rate in west java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_Ind_JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation rate in central java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_Ind_JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation rate in south sulawesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_Ind_SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation rate in east java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF_Ind_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domestic flights jakarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_Ind_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domestic flights east java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_Ind_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domestic flights south sulawesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF_Ind_SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int_F_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">international flights jakarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int_F_Ind_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int_F_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">international flights east java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int_F_Ind_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign visitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign_vis_Ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotel occupancy Jakarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_Ind_JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1g9OeNpLuXKhCqu7EqZSfP5XLvWBKquhr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotel occupancy west java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_Ind_JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotel occupancy central java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_Ind_JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotel occupancy east java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_Ind_JI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotel occupancy south sulawesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO_Ind_SN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -911,7 +910,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -934,7 +948,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -942,358 +956,99 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="58.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="48" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" customFormat="false" ht="51" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1371,7 +1126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" s="4" customFormat="true" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" s="4" customFormat="true" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1423,7 +1178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" s="4" customFormat="true" ht="51" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1449,7 +1204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" customFormat="false" ht="102" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1475,7 +1230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1501,7 +1256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" s="4" customFormat="true" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
@@ -1527,7 +1282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1553,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>47</v>
       </c>
@@ -1579,7 +1334,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1603,7 +1358,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1629,11 +1384,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1642,10 +1397,10 @@
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -1655,11 +1410,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1668,10 +1423,10 @@
       <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -1681,7 +1436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="51" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1705,7 +1460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" s="4" customFormat="true" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1482,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -1747,7 +1502,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>71</v>
       </c>
@@ -1766,7 +1521,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -1788,7 +1543,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1810,7 +1565,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
@@ -1832,11 +1587,11 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1845,40 +1600,40 @@
       <c r="D23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1887,7 +1642,7 @@
       <c r="D25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1896,11 +1651,11 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1909,18 +1664,18 @@
       <c r="D26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1929,7 +1684,7 @@
       <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1938,11 +1693,11 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1951,7 +1706,7 @@
       <c r="D28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>87</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -1960,11 +1715,11 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1973,7 +1728,7 @@
       <c r="D29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -1982,11 +1737,11 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1995,18 +1750,18 @@
       <c r="D30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="0" t="s">
         <v>93</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" s="4" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -2015,7 +1770,7 @@
       <c r="D31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -2024,11 +1779,11 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2050,11 +1805,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -2074,11 +1829,11 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -2100,11 +1855,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -2126,11 +1881,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -2152,11 +1907,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -2178,11 +1933,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -2202,11 +1957,11 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -2225,11 +1980,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -2248,11 +2003,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" s="4" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -2272,11 +2027,11 @@
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -2295,11 +2050,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -2318,11 +2073,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -2341,11 +2096,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -2364,11 +2119,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -2387,11 +2142,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -2410,11 +2165,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -2436,11 +2191,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -2462,11 +2217,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -2488,7 +2243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="51" customFormat="false" ht="51" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
@@ -2512,23 +2267,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G52" s="5" t="s">
@@ -2538,11 +2293,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -2551,10 +2306,10 @@
       <c r="D53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G53" s="5" t="s">
@@ -2564,11 +2319,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -2577,10 +2332,10 @@
       <c r="D54" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G54" s="5" t="s">
@@ -2590,11 +2345,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -2603,10 +2358,10 @@
       <c r="D55" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -2616,20 +2371,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B56" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="0" t="s">
         <v>29</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -2642,11 +2397,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57" customFormat="false" ht="102" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -2655,10 +2410,10 @@
       <c r="D57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G57" s="5" t="s">
@@ -2668,7 +2423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="58" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
         <v>34</v>
       </c>
@@ -2694,11 +2449,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -2710,7 +2465,7 @@
       <c r="E59" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G59" s="5" t="s">
@@ -2720,23 +2475,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B60" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G60" s="5" t="s">
@@ -2746,11 +2501,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -2759,10 +2514,10 @@
       <c r="D61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G61" s="5" t="s">
@@ -2772,7 +2527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="62" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
         <v>51</v>
       </c>
@@ -2798,11 +2553,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -2811,10 +2566,10 @@
       <c r="D63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G63" s="1" t="s">
@@ -2824,11 +2579,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -2837,10 +2592,10 @@
       <c r="D64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G64" s="5" t="s">
@@ -2850,11 +2605,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -2863,10 +2618,10 @@
       <c r="D65" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G65" s="5" t="s">
@@ -2876,11 +2631,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="66" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -2889,10 +2644,10 @@
       <c r="D66" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G66" s="5" t="s">
@@ -2902,11 +2657,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="67" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -2915,10 +2670,10 @@
       <c r="D67" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G67" s="5" t="s">
@@ -2928,11 +2683,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="68" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -2941,10 +2696,10 @@
       <c r="D68" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G68" s="5" t="s">
@@ -2954,11 +2709,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="69" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -2967,10 +2722,10 @@
       <c r="D69" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G69" s="5" t="s">
@@ -2980,11 +2735,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="70" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="4" t="s">
@@ -2993,10 +2748,10 @@
       <c r="D70" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G70" s="5" t="s">
@@ -3006,11 +2761,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="71" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -3019,10 +2774,10 @@
       <c r="D71" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G71" s="5" t="s">
@@ -3032,11 +2787,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="72" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -3045,10 +2800,10 @@
       <c r="D72" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G72" s="5" t="s">
@@ -3058,11 +2813,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -3071,10 +2826,10 @@
       <c r="D73" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G73" s="5" t="s">
@@ -3084,11 +2839,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -3097,10 +2852,10 @@
       <c r="D74" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G74" s="5" t="s">
@@ -3110,11 +2865,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="75" customFormat="false" ht="38.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="4" t="s">
@@ -3123,10 +2878,10 @@
       <c r="D75" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G75" s="5" t="s">
@@ -3136,11 +2891,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="76" customFormat="false" ht="89.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -3149,10 +2904,10 @@
       <c r="D76" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G76" s="5" t="s">
@@ -3162,11 +2917,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="77" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -3175,10 +2930,10 @@
       <c r="D77" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G77" s="1" t="s">
@@ -3188,11 +2943,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="78" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -3201,10 +2956,10 @@
       <c r="D78" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G78" s="5" t="s">
@@ -3214,11 +2969,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="79" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -3227,10 +2982,10 @@
       <c r="D79" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G79" s="5" t="s">
@@ -3240,11 +2995,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="80" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -3253,10 +3008,10 @@
       <c r="D80" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G80" s="5" t="s">
@@ -3266,11 +3021,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="81" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -3279,10 +3034,10 @@
       <c r="D81" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G81" s="5" t="s">
@@ -3292,11 +3047,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="82" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -3305,10 +3060,10 @@
       <c r="D82" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G82" s="5" t="s">
@@ -3318,11 +3073,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="83" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -3331,10 +3086,10 @@
       <c r="D83" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G83" s="5" t="s">
@@ -3344,11 +3099,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="84" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="4" t="s">
@@ -3357,10 +3112,10 @@
       <c r="D84" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G84" s="5" t="s">
@@ -3370,11 +3125,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="85" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -3383,10 +3138,10 @@
       <c r="D85" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G85" s="5" t="s">
@@ -3396,11 +3151,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="86" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -3409,10 +3164,10 @@
       <c r="D86" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G86" s="5" t="s">
@@ -3422,11 +3177,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="87" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C87" s="4" t="s">
@@ -3435,10 +3190,10 @@
       <c r="D87" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G87" s="5" t="s">
@@ -3448,11 +3203,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="88" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -3461,10 +3216,10 @@
       <c r="D88" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G88" s="5" t="s">
@@ -3474,11 +3229,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="89" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -3487,10 +3242,10 @@
       <c r="D89" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G89" s="5" t="s">
@@ -3500,11 +3255,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="90" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C90" s="4" t="s">
@@ -3513,10 +3268,10 @@
       <c r="D90" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G90" s="5" t="s">
@@ -3526,11 +3281,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="91" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C91" s="4" t="s">
@@ -3539,10 +3294,10 @@
       <c r="D91" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G91" s="5" t="s">
@@ -3552,11 +3307,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="92" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C92" s="4" t="s">
@@ -3565,10 +3320,10 @@
       <c r="D92" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G92" s="5" t="s">
@@ -3578,11 +3333,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="93" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C93" s="4" t="s">
@@ -3591,10 +3346,10 @@
       <c r="D93" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G93" s="5" t="s">
@@ -3604,11 +3359,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="94" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -3617,10 +3372,10 @@
       <c r="D94" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G94" s="5" t="s">
@@ -3630,11 +3385,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="95" customFormat="false" ht="63.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -3643,10 +3398,10 @@
       <c r="D95" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="0" t="s">
         <v>148</v>
       </c>
       <c r="G95" s="5" t="s">
@@ -3656,7 +3411,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
         <v>8</v>
       </c>
@@ -3682,7 +3437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>24</v>
       </c>
@@ -3708,7 +3463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="98" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
         <v>71</v>
       </c>
@@ -3734,7 +3489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="99" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
         <v>34</v>
       </c>
@@ -3760,7 +3515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="100" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
         <v>39</v>
       </c>
@@ -3786,7 +3541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="101" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
         <v>43</v>
       </c>
@@ -3812,7 +3567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="102" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
         <v>51</v>
       </c>
@@ -3836,7 +3591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="103" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
         <v>225</v>
       </c>
@@ -3862,8 +3617,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="104" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>229</v>
       </c>
       <c r="B104" s="4" t="s">
@@ -3873,21 +3628,21 @@
         <v>65</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E104" t="s">
-        <v>245</v>
+        <v>230</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>231</v>
       </c>
       <c r="F104" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>233</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>9</v>
@@ -3896,21 +3651,21 @@
         <v>65</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E105" t="s">
-        <v>246</v>
+        <v>234</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>235</v>
       </c>
       <c r="F105" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>236</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>9</v>
@@ -3919,21 +3674,21 @@
         <v>65</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E106" t="s">
-        <v>247</v>
+        <v>237</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="F106" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>239</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>9</v>
@@ -3942,21 +3697,21 @@
         <v>65</v>
       </c>
       <c r="D107" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
         <v>242</v>
-      </c>
-      <c r="E107" t="s">
-        <v>244</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>233</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>9</v>
@@ -3967,19 +3722,19 @@
       <c r="D108" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E108" t="s">
-        <v>248</v>
+      <c r="E108" s="0" t="s">
+        <v>244</v>
       </c>
       <c r="F108" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>234</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>9</v>
@@ -3988,10 +3743,10 @@
         <v>65</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E109" t="s">
-        <v>255</v>
+        <v>246</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>247</v>
       </c>
       <c r="F109" s="4" t="s">
         <v>70</v>
@@ -4000,9 +3755,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>235</v>
+    <row r="110" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>248</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>9</v>
@@ -4011,10 +3766,10 @@
         <v>65</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E110" t="s">
-        <v>256</v>
+        <v>249</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>250</v>
       </c>
       <c r="F110" s="4" t="s">
         <v>70</v>
@@ -4023,9 +3778,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>236</v>
+    <row r="111" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>251</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>9</v>
@@ -4036,8 +3791,8 @@
       <c r="D111" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E111" t="s">
-        <v>259</v>
+      <c r="E111" s="0" t="s">
+        <v>253</v>
       </c>
       <c r="F111" s="4" t="s">
         <v>70</v>
@@ -4046,9 +3801,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>237</v>
+    <row r="112" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>254</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>9</v>
@@ -4057,10 +3812,10 @@
         <v>65</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E112" t="s">
-        <v>257</v>
+        <v>255</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>256</v>
       </c>
       <c r="F112" s="4" t="s">
         <v>70</v>
@@ -4069,9 +3824,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>238</v>
+    <row r="113" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>257</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>9</v>
@@ -4080,10 +3835,10 @@
         <v>65</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E113" t="s">
         <v>258</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>259</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>70</v>
@@ -4092,8 +3847,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="114" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
         <v>260</v>
       </c>
       <c r="B114" s="4" t="s">
@@ -4103,18 +3858,18 @@
         <v>65</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E114" t="s">
-        <v>277</v>
+        <v>261</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>262</v>
       </c>
       <c r="F114" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>261</v>
+    <row r="115" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>263</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>9</v>
@@ -4123,21 +3878,21 @@
         <v>65</v>
       </c>
       <c r="D115" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="E115" t="s">
-        <v>271</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>262</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>9</v>
@@ -4148,19 +3903,19 @@
       <c r="D116" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E116" t="s">
-        <v>272</v>
+      <c r="E116" s="0" t="s">
+        <v>269</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>263</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>270</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>9</v>
@@ -4169,21 +3924,21 @@
         <v>65</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E117" t="s">
+        <v>271</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>273</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>264</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>9</v>
@@ -4192,21 +3947,21 @@
         <v>65</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E118" t="s">
         <v>274</v>
       </c>
+      <c r="E118" s="0" t="s">
+        <v>275</v>
+      </c>
       <c r="F118" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>276</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>9</v>
@@ -4215,72 +3970,80 @@
         <v>65</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E119" t="s">
-        <v>275</v>
+        <v>277</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>278</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H119">
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Santiago"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G62" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G64" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G65" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G66" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G67" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G68" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G69" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G70" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G71" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G72" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G73" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G74" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G75" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G76" r:id="rId25" display="Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G78" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G79" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G80" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G81" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G82" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G83" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G84" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G85" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G86" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G87" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G88" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G89" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G90" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G91" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G92" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G93" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G94" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="G95" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="G98" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="G101" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8"/>
+    <hyperlink ref="G4" r:id="rId3" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G6" r:id="rId4" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G9" r:id="rId6" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G10" r:id="rId7" display="https://github.com/MinCiencia/Datos-COVID19/blob/master/output/producto5/TotalesNacionales.csv"/>
+    <hyperlink ref="G11" r:id="rId8" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto8"/>
+    <hyperlink ref="G13" r:id="rId9" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto20"/>
+    <hyperlink ref="G14" r:id="rId10" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto7"/>
+    <hyperlink ref="G15" r:id="rId11" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto40"/>
+    <hyperlink ref="G62" r:id="rId12" display="Assembled from various public announcements, compiled here&#10;https://docs.google.com/spreadsheets/d/1EeeSJE7jzTyf-w6ESXhN58rfIme0wiU1EpOKtbYeEQ8/edit?usp=sharing"/>
+    <hyperlink ref="G64" r:id="rId13" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G65" r:id="rId14" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G66" r:id="rId15" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G67" r:id="rId16" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G68" r:id="rId17" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G69" r:id="rId18" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G70" r:id="rId19" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G71" r:id="rId20" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G72" r:id="rId21" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G73" r:id="rId22" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G74" r:id="rId23" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G75" r:id="rId24" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G76" r:id="rId25" display="Quarterly Disclosure (Divulgação trimestral), Tabelas por Unidade da Federação (Tables by Federation Unit), Table 33 (Rio de Janeiro): https://www.ibge.gov.br/estatisticas/multidominio/condicoes-de-vida-desigualdade-e-pobreza/9173-pesquisa-nacional-por-amostra-de-domicilios-continua-trimestral.html?edicao=28690&amp;t=resultados"/>
+    <hyperlink ref="G78" r:id="rId26" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G79" r:id="rId27" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G80" r:id="rId28" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G81" r:id="rId29" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G82" r:id="rId30" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G83" r:id="rId31" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G84" r:id="rId32" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G85" r:id="rId33" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G86" r:id="rId34" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G87" r:id="rId35" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G88" r:id="rId36" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G89" r:id="rId37" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G90" r:id="rId38" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G91" r:id="rId39" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G92" r:id="rId40" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G93" r:id="rId41" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G94" r:id="rId42" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G95" r:id="rId43" display="https://www.data.rio/datasets/qualidade-do-ar-dados-hor%C3%A1rios"/>
+    <hyperlink ref="G98" r:id="rId44" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53"/>
+    <hyperlink ref="G101" r:id="rId45" display="https://github.com/MinCiencia/Datos-COVID19/tree/master/output/producto53"/>
   </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId46"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>